<commit_message>
Reset log & push
</commit_message>
<xml_diff>
--- a/Final_pjt2/WBS.xlsx
+++ b/Final_pjt2/WBS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Genia\Final_pjt2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D80E07A-43C4-44DF-B262-B7E60424A810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A0558AA-904F-4CE5-A2C1-C27F2A0DC151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4620" yWindow="2025" windowWidth="20235" windowHeight="17760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4620" yWindow="2025" windowWidth="30645" windowHeight="17760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WBS" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="78">
   <si>
     <t>테스트</t>
   </si>
@@ -206,10 +206,6 @@
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>코드 병합</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">진행율 기준일자 : </t>
   </si>
   <si>
@@ -321,6 +317,14 @@
   </si>
   <si>
     <t>Text Feature Test &amp; Extraction</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>시스템 테스트</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dash 코드 병합 및 모듈화</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -552,7 +556,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="88">
+  <borders count="97">
     <border>
       <left/>
       <right/>
@@ -1639,13 +1643,144 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="slantDashDot">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="slantDashDot">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="slantDashDot">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="slantDashDot">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="slantDashDot">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="slantDashDot">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="slantDashDot">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="slantDashDot">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="slantDashDot">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="slantDashDot">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="slantDashDot">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="slantDashDot">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="216">
+  <cellXfs count="244">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2030,6 +2165,90 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="24" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="85" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="86" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="79" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="10" borderId="76" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="10" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="10" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="9" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="9" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="10" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="10" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="10" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="10" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="11" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2063,89 +2282,53 @@
     <xf numFmtId="176" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="85" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="86" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="79" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="10" borderId="76" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="10" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="10" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="9" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="9" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="10" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="10" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="10" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="10" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2162,12 +2345,6 @@
     <xf numFmtId="0" fontId="8" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2183,21 +2360,12 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="16" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2228,39 +2396,6 @@
     <xf numFmtId="0" fontId="8" fillId="15" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="17" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2282,17 +2417,101 @@
     <xf numFmtId="0" fontId="8" fillId="21" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="34" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="34" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="34" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="34" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="90" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="91" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="92" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="93" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="92" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="93" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="92" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="93" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="92" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="93" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="92" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="93" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="94" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="95" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="96" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2633,9 +2852,9 @@
   </tableStyles>
   <colors>
     <mruColors>
+      <color rgb="FFFF8F8F"/>
       <color rgb="FFFFFFCC"/>
       <color rgb="FFFFFF69"/>
-      <color rgb="FFFF8F8F"/>
       <color rgb="FF33FF8F"/>
       <color rgb="FFFFFF99"/>
     </mruColors>
@@ -2975,8 +3194,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3011,21 +3230,21 @@
     </row>
     <row r="2" spans="1:13" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="55"/>
-      <c r="B2" s="139" t="s">
+      <c r="B2" s="128" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="140"/>
-      <c r="D2" s="140"/>
-      <c r="E2" s="140"/>
+      <c r="C2" s="129"/>
+      <c r="D2" s="129"/>
+      <c r="E2" s="129"/>
       <c r="F2" s="106"/>
       <c r="G2" s="106"/>
       <c r="H2" s="106"/>
       <c r="I2" s="106" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J2" s="107">
         <f ca="1">TODAY()</f>
-        <v>45264</v>
+        <v>45272</v>
       </c>
       <c r="K2" s="108" t="s">
         <v>31</v>
@@ -3038,44 +3257,44 @@
     </row>
     <row r="3" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="87"/>
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="140" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="153" t="s">
+      <c r="C3" s="142" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="155" t="s">
+      <c r="D3" s="144" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="157" t="s">
+      <c r="E3" s="146" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="158"/>
-      <c r="G3" s="158"/>
-      <c r="H3" s="158"/>
-      <c r="I3" s="159"/>
-      <c r="J3" s="128" t="s">
+      <c r="F3" s="147"/>
+      <c r="G3" s="147"/>
+      <c r="H3" s="147"/>
+      <c r="I3" s="148"/>
+      <c r="J3" s="156" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="144" t="s">
+      <c r="K3" s="133" t="s">
         <v>27</v>
       </c>
-      <c r="L3" s="145"/>
+      <c r="L3" s="134"/>
       <c r="M3" s="30"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="87"/>
-      <c r="B4" s="152"/>
-      <c r="C4" s="154"/>
-      <c r="D4" s="156"/>
-      <c r="E4" s="160"/>
-      <c r="F4" s="161"/>
-      <c r="G4" s="161"/>
-      <c r="H4" s="161"/>
-      <c r="I4" s="162"/>
-      <c r="J4" s="129"/>
-      <c r="K4" s="146"/>
-      <c r="L4" s="147"/>
+      <c r="B4" s="141"/>
+      <c r="C4" s="143"/>
+      <c r="D4" s="145"/>
+      <c r="E4" s="149"/>
+      <c r="F4" s="150"/>
+      <c r="G4" s="150"/>
+      <c r="H4" s="150"/>
+      <c r="I4" s="151"/>
+      <c r="J4" s="157"/>
+      <c r="K4" s="135"/>
+      <c r="L4" s="136"/>
     </row>
     <row r="5" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="87"/>
@@ -3099,7 +3318,7 @@
       <c r="I5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="130"/>
+      <c r="J5" s="158"/>
       <c r="K5" s="84" t="s">
         <v>6</v>
       </c>
@@ -3109,10 +3328,10 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="87"/>
-      <c r="B6" s="165" t="s">
+      <c r="B6" s="154" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="166"/>
+      <c r="C6" s="155"/>
       <c r="D6" s="16"/>
       <c r="E6" s="17" t="str">
         <f>CONCATENATE(NETWORKDAYS(F6,G6),"일")</f>
@@ -3143,15 +3362,15 @@
       </c>
       <c r="L6" s="31">
         <f t="shared" ref="L6:L28" ca="1" si="0">IF(G6-$J$2&lt;=0,0,G6-$J$2)</f>
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="87"/>
-      <c r="B7" s="131" t="s">
+      <c r="B7" s="159" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="132"/>
+      <c r="C7" s="160"/>
       <c r="D7" s="13"/>
       <c r="E7" s="13" t="str">
         <f>CONCATENATE(NETWORKDAYS(F7,G7),"일")</f>
@@ -3181,13 +3400,13 @@
       </c>
       <c r="L7" s="32">
         <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="M7" s="36"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="87"/>
-      <c r="B8" s="133" t="s">
+      <c r="B8" s="161" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="54" t="s">
@@ -3219,12 +3438,12 @@
       </c>
       <c r="L8" s="33">
         <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="87"/>
-      <c r="B9" s="134"/>
+      <c r="B9" s="162"/>
       <c r="C9" s="3" t="s">
         <v>21</v>
       </c>
@@ -3245,7 +3464,7 @@
         <v>10</v>
       </c>
       <c r="I9" s="11">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="J9" s="66"/>
       <c r="K9" s="59">
@@ -3259,12 +3478,12 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="87"/>
-      <c r="B10" s="134"/>
+      <c r="B10" s="162"/>
       <c r="C10" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="E10" s="6" t="str">
         <f t="shared" si="1"/>
@@ -3280,7 +3499,7 @@
         <v>10</v>
       </c>
       <c r="I10" s="11">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="J10" s="66"/>
       <c r="K10" s="59">
@@ -3294,7 +3513,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="87"/>
-      <c r="B11" s="134"/>
+      <c r="B11" s="162"/>
       <c r="C11" s="3" t="s">
         <v>41</v>
       </c>
@@ -3329,7 +3548,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="87"/>
-      <c r="B12" s="134"/>
+      <c r="B12" s="162"/>
       <c r="C12" s="3" t="s">
         <v>42</v>
       </c>
@@ -3364,7 +3583,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="87"/>
-      <c r="B13" s="134"/>
+      <c r="B13" s="162"/>
       <c r="C13" s="94" t="s">
         <v>45</v>
       </c>
@@ -3399,9 +3618,9 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="87"/>
-      <c r="B14" s="134"/>
+      <c r="B14" s="162"/>
       <c r="C14" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D14" s="90" t="s">
         <v>11</v>
@@ -3416,7 +3635,7 @@
       <c r="G14" s="20">
         <v>45258</v>
       </c>
-      <c r="H14" s="136" t="s">
+      <c r="H14" s="164" t="s">
         <v>2</v>
       </c>
       <c r="I14" s="91">
@@ -3434,9 +3653,9 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="87"/>
-      <c r="B15" s="134"/>
+      <c r="B15" s="162"/>
       <c r="C15" s="94" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D15" s="90" t="s">
         <v>32</v>
@@ -3451,9 +3670,9 @@
       <c r="G15" s="20">
         <v>45258</v>
       </c>
-      <c r="H15" s="137"/>
+      <c r="H15" s="165"/>
       <c r="I15" s="91">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="J15" s="68"/>
       <c r="K15" s="92">
@@ -3467,9 +3686,9 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="87"/>
-      <c r="B16" s="135"/>
+      <c r="B16" s="163"/>
       <c r="C16" s="53" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D16" s="90" t="s">
         <v>11</v>
@@ -3484,9 +3703,9 @@
       <c r="G16" s="20">
         <v>45258</v>
       </c>
-      <c r="H16" s="138"/>
+      <c r="H16" s="166"/>
       <c r="I16" s="91">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="J16" s="68"/>
       <c r="K16" s="92">
@@ -3500,10 +3719,10 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="87"/>
-      <c r="B17" s="131" t="s">
+      <c r="B17" s="159" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="132"/>
+      <c r="C17" s="160"/>
       <c r="D17" s="21"/>
       <c r="E17" s="21" t="str">
         <f>CONCATENATE(NETWORKDAYS(F17,G17),"일")</f>
@@ -3531,16 +3750,16 @@
       </c>
       <c r="L17" s="34">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="87"/>
-      <c r="B18" s="148" t="s">
+      <c r="B18" s="137" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="213" t="s">
-        <v>75</v>
+      <c r="C18" s="212" t="s">
+        <v>74</v>
       </c>
       <c r="D18" s="52" t="s">
         <v>11</v>
@@ -3559,7 +3778,7 @@
         <v>37</v>
       </c>
       <c r="I18" s="11">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="J18" s="66"/>
       <c r="K18" s="59">
@@ -3568,13 +3787,13 @@
       </c>
       <c r="L18" s="33">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="87"/>
-      <c r="B19" s="149"/>
-      <c r="C19" s="214"/>
+      <c r="B19" s="138"/>
+      <c r="C19" s="213"/>
       <c r="D19" s="52" t="s">
         <v>11</v>
       </c>
@@ -3592,7 +3811,7 @@
         <v>12</v>
       </c>
       <c r="I19" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19" s="66"/>
       <c r="K19" s="59">
@@ -3606,8 +3825,8 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="87"/>
-      <c r="B20" s="149"/>
-      <c r="C20" s="214"/>
+      <c r="B20" s="138"/>
+      <c r="C20" s="213"/>
       <c r="D20" s="49" t="s">
         <v>11</v>
       </c>
@@ -3625,7 +3844,7 @@
         <v>5</v>
       </c>
       <c r="I20" s="11">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="J20" s="66"/>
       <c r="K20" s="59">
@@ -3634,13 +3853,13 @@
       </c>
       <c r="L20" s="33">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="87"/>
-      <c r="B21" s="149"/>
-      <c r="C21" s="215"/>
+      <c r="B21" s="138"/>
+      <c r="C21" s="214"/>
       <c r="D21" s="49" t="s">
         <v>11</v>
       </c>
@@ -3658,7 +3877,7 @@
         <v>38</v>
       </c>
       <c r="I21" s="11">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="J21" s="66"/>
       <c r="K21" s="59">
@@ -3667,14 +3886,14 @@
       </c>
       <c r="L21" s="33">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A22" s="87"/>
-      <c r="B22" s="149"/>
-      <c r="C22" s="212" t="s">
-        <v>76</v>
+      <c r="B22" s="138"/>
+      <c r="C22" s="215" t="s">
+        <v>75</v>
       </c>
       <c r="D22" s="49" t="s">
         <v>11</v>
@@ -3693,7 +3912,7 @@
         <v>2</v>
       </c>
       <c r="I22" s="11">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="J22" s="66"/>
       <c r="K22" s="59">
@@ -3702,27 +3921,27 @@
       </c>
       <c r="L22" s="33">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="87"/>
-      <c r="B23" s="149"/>
-      <c r="C23" s="163" t="s">
+      <c r="B23" s="138"/>
+      <c r="C23" s="152" t="s">
         <v>46</v>
       </c>
       <c r="D23" s="49" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E23" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>11일</v>
+        <v>3일</v>
       </c>
       <c r="F23" s="1">
-        <v>45259</v>
+        <v>45273</v>
       </c>
       <c r="G23" s="1">
-        <v>45273</v>
+        <v>45275</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>2</v>
@@ -3737,15 +3956,15 @@
       </c>
       <c r="L23" s="33">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="87"/>
-      <c r="B24" s="149"/>
-      <c r="C24" s="164"/>
+      <c r="B24" s="138"/>
+      <c r="C24" s="153"/>
       <c r="D24" s="6" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E24" s="5" t="str">
         <f t="shared" si="1"/>
@@ -3770,14 +3989,14 @@
       </c>
       <c r="L24" s="33">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="87"/>
-      <c r="B25" s="150"/>
+      <c r="B25" s="139"/>
       <c r="C25" s="53" t="s">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>6</v>
@@ -3805,7 +4024,7 @@
       </c>
       <c r="L25" s="33">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
@@ -3843,7 +4062,7 @@
       </c>
       <c r="L26" s="34">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3852,7 +4071,7 @@
         <v>44</v>
       </c>
       <c r="C27" s="50" t="s">
-        <v>24</v>
+        <v>76</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>6</v>
@@ -3880,7 +4099,7 @@
       </c>
       <c r="L27" s="35">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
@@ -3918,12 +4137,12 @@
       </c>
       <c r="L28" s="34">
         <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="87"/>
-      <c r="B29" s="141" t="s">
+      <c r="B29" s="130" t="s">
         <v>25</v>
       </c>
       <c r="C29" s="50" t="s">
@@ -3955,12 +4174,12 @@
       </c>
       <c r="L29" s="37">
         <f ca="1">IF(G30-$J$2&lt;=0,0,G30-$J$2)</f>
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="87"/>
-      <c r="B30" s="142"/>
+      <c r="B30" s="131"/>
       <c r="C30" s="51" t="s">
         <v>23</v>
       </c>
@@ -3990,12 +4209,12 @@
       </c>
       <c r="L30" s="33">
         <f ca="1">IF(G31-$J$2&lt;=0,0,G31-$J$2)</f>
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="55"/>
-      <c r="B31" s="143"/>
+      <c r="B31" s="132"/>
       <c r="C31" s="73" t="s">
         <v>7</v>
       </c>
@@ -4025,7 +4244,7 @@
       </c>
       <c r="L31" s="81">
         <f ca="1">IF(G31-$J$2&lt;=0,0,G31-$J$2)</f>
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -4079,7 +4298,7 @@
       <formula>NOT(ISERROR(SEARCH("전혁선",H6)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I8:I16 I27 I29:I31 I18:I25">
+  <conditionalFormatting sqref="I8:I16 I18:I25 I27 I29:I31">
     <cfRule type="cellIs" dxfId="8" priority="23" operator="between">
       <formula>0.01</formula>
       <formula>0.69</formula>
@@ -4110,8 +4329,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B3:AH19"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="T22" sqref="T22"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="AL22" sqref="AL22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4122,140 +4341,140 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B3" s="174" t="s">
+      <c r="B3" s="188" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="176" t="s">
+      <c r="C3" s="190" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="176"/>
-      <c r="E3" s="194" t="s">
+      <c r="D3" s="190"/>
+      <c r="E3" s="171" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="195"/>
-      <c r="G3" s="195"/>
-      <c r="H3" s="195"/>
-      <c r="I3" s="195"/>
-      <c r="J3" s="195"/>
-      <c r="K3" s="195"/>
-      <c r="L3" s="195"/>
-      <c r="M3" s="195"/>
-      <c r="N3" s="195"/>
-      <c r="O3" s="195"/>
-      <c r="P3" s="195"/>
-      <c r="Q3" s="195"/>
-      <c r="R3" s="195"/>
-      <c r="S3" s="195"/>
-      <c r="T3" s="195"/>
-      <c r="U3" s="195"/>
-      <c r="V3" s="195"/>
-      <c r="W3" s="195"/>
-      <c r="X3" s="195"/>
-      <c r="Y3" s="195"/>
-      <c r="Z3" s="195"/>
-      <c r="AA3" s="195"/>
-      <c r="AB3" s="195"/>
-      <c r="AC3" s="195"/>
-      <c r="AD3" s="195"/>
-      <c r="AE3" s="195"/>
-      <c r="AF3" s="195"/>
-      <c r="AG3" s="195"/>
-      <c r="AH3" s="196"/>
+      <c r="F3" s="172"/>
+      <c r="G3" s="172"/>
+      <c r="H3" s="172"/>
+      <c r="I3" s="172"/>
+      <c r="J3" s="172"/>
+      <c r="K3" s="172"/>
+      <c r="L3" s="172"/>
+      <c r="M3" s="172"/>
+      <c r="N3" s="172"/>
+      <c r="O3" s="172"/>
+      <c r="P3" s="172"/>
+      <c r="Q3" s="172"/>
+      <c r="R3" s="172"/>
+      <c r="S3" s="172"/>
+      <c r="T3" s="172"/>
+      <c r="U3" s="172"/>
+      <c r="V3" s="172"/>
+      <c r="W3" s="172"/>
+      <c r="X3" s="172"/>
+      <c r="Y3" s="172"/>
+      <c r="Z3" s="172"/>
+      <c r="AA3" s="172"/>
+      <c r="AB3" s="172"/>
+      <c r="AC3" s="172"/>
+      <c r="AD3" s="172"/>
+      <c r="AE3" s="172"/>
+      <c r="AF3" s="172"/>
+      <c r="AG3" s="172"/>
+      <c r="AH3" s="173"/>
     </row>
     <row r="4" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B4" s="175"/>
-      <c r="C4" s="177"/>
-      <c r="D4" s="178"/>
-      <c r="E4" s="197" t="s">
+      <c r="B4" s="189"/>
+      <c r="C4" s="191"/>
+      <c r="D4" s="192"/>
+      <c r="E4" s="174" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="198"/>
-      <c r="G4" s="198"/>
-      <c r="H4" s="198"/>
-      <c r="I4" s="198"/>
-      <c r="J4" s="198"/>
-      <c r="K4" s="198"/>
-      <c r="L4" s="198"/>
-      <c r="M4" s="198"/>
-      <c r="N4" s="198"/>
-      <c r="O4" s="198"/>
-      <c r="P4" s="198"/>
-      <c r="Q4" s="198"/>
-      <c r="R4" s="198"/>
-      <c r="S4" s="198"/>
-      <c r="T4" s="198"/>
-      <c r="U4" s="198"/>
-      <c r="V4" s="198"/>
-      <c r="W4" s="198"/>
-      <c r="X4" s="198"/>
-      <c r="Y4" s="198"/>
-      <c r="Z4" s="198"/>
-      <c r="AA4" s="198"/>
-      <c r="AB4" s="198"/>
-      <c r="AC4" s="198"/>
-      <c r="AD4" s="198"/>
-      <c r="AE4" s="198"/>
-      <c r="AF4" s="198"/>
-      <c r="AG4" s="198"/>
-      <c r="AH4" s="199"/>
-    </row>
-    <row r="5" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B5" s="187" t="s">
+      <c r="F4" s="175"/>
+      <c r="G4" s="175"/>
+      <c r="H4" s="175"/>
+      <c r="I4" s="175"/>
+      <c r="J4" s="175"/>
+      <c r="K4" s="175"/>
+      <c r="L4" s="175"/>
+      <c r="M4" s="175"/>
+      <c r="N4" s="175"/>
+      <c r="O4" s="175"/>
+      <c r="P4" s="175"/>
+      <c r="Q4" s="175"/>
+      <c r="R4" s="175"/>
+      <c r="S4" s="175"/>
+      <c r="T4" s="175"/>
+      <c r="U4" s="175"/>
+      <c r="V4" s="175"/>
+      <c r="W4" s="175"/>
+      <c r="X4" s="175"/>
+      <c r="Y4" s="175"/>
+      <c r="Z4" s="175"/>
+      <c r="AA4" s="175"/>
+      <c r="AB4" s="175"/>
+      <c r="AC4" s="175"/>
+      <c r="AD4" s="175"/>
+      <c r="AE4" s="175"/>
+      <c r="AF4" s="175"/>
+      <c r="AG4" s="175"/>
+      <c r="AH4" s="176"/>
+    </row>
+    <row r="5" spans="2:34" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="198" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="188"/>
-      <c r="D5" s="189"/>
-      <c r="E5" s="183">
+      <c r="C5" s="199"/>
+      <c r="D5" s="200"/>
+      <c r="E5" s="178">
         <v>1</v>
       </c>
-      <c r="F5" s="201"/>
-      <c r="G5" s="201"/>
-      <c r="H5" s="201"/>
-      <c r="I5" s="202"/>
-      <c r="J5" s="203">
+      <c r="F5" s="179"/>
+      <c r="G5" s="179"/>
+      <c r="H5" s="179"/>
+      <c r="I5" s="180"/>
+      <c r="J5" s="181">
         <v>2</v>
       </c>
-      <c r="K5" s="198"/>
-      <c r="L5" s="198"/>
-      <c r="M5" s="198"/>
-      <c r="N5" s="199"/>
-      <c r="O5" s="200">
+      <c r="K5" s="175"/>
+      <c r="L5" s="175"/>
+      <c r="M5" s="175"/>
+      <c r="N5" s="176"/>
+      <c r="O5" s="177">
         <v>3</v>
       </c>
-      <c r="P5" s="198"/>
-      <c r="Q5" s="198"/>
-      <c r="R5" s="198"/>
-      <c r="S5" s="199"/>
-      <c r="T5" s="200">
+      <c r="P5" s="175"/>
+      <c r="Q5" s="175"/>
+      <c r="R5" s="175"/>
+      <c r="S5" s="176"/>
+      <c r="T5" s="224">
         <v>4</v>
       </c>
-      <c r="U5" s="198"/>
-      <c r="V5" s="198"/>
-      <c r="W5" s="198"/>
-      <c r="X5" s="199"/>
-      <c r="Y5" s="200">
+      <c r="U5" s="225"/>
+      <c r="V5" s="225"/>
+      <c r="W5" s="225"/>
+      <c r="X5" s="226"/>
+      <c r="Y5" s="177">
         <v>5</v>
       </c>
-      <c r="Z5" s="198"/>
-      <c r="AA5" s="198"/>
-      <c r="AB5" s="198"/>
-      <c r="AC5" s="199"/>
-      <c r="AD5" s="204">
+      <c r="Z5" s="175"/>
+      <c r="AA5" s="175"/>
+      <c r="AB5" s="175"/>
+      <c r="AC5" s="176"/>
+      <c r="AD5" s="182">
         <v>6</v>
       </c>
-      <c r="AE5" s="201"/>
-      <c r="AF5" s="201"/>
-      <c r="AG5" s="201"/>
-      <c r="AH5" s="202"/>
+      <c r="AE5" s="179"/>
+      <c r="AF5" s="179"/>
+      <c r="AG5" s="179"/>
+      <c r="AH5" s="180"/>
     </row>
     <row r="6" spans="2:34" x14ac:dyDescent="0.3">
       <c r="B6" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="179" t="s">
+      <c r="C6" s="169" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="180"/>
+      <c r="D6" s="170"/>
       <c r="E6" s="47"/>
       <c r="F6" s="47"/>
       <c r="G6" s="47"/>
@@ -4270,12 +4489,12 @@
       <c r="P6" s="27"/>
       <c r="Q6" s="27"/>
       <c r="R6" s="27"/>
-      <c r="S6" s="41"/>
-      <c r="T6" s="40"/>
-      <c r="U6" s="27"/>
-      <c r="V6" s="27"/>
-      <c r="W6" s="27"/>
-      <c r="X6" s="41"/>
+      <c r="S6" s="218"/>
+      <c r="T6" s="228"/>
+      <c r="U6" s="229"/>
+      <c r="V6" s="229"/>
+      <c r="W6" s="229"/>
+      <c r="X6" s="230"/>
       <c r="Y6" s="40"/>
       <c r="Z6" s="27"/>
       <c r="AA6" s="27"/>
@@ -4291,10 +4510,10 @@
       <c r="B7" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="179" t="s">
+      <c r="C7" s="169" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="180"/>
+      <c r="D7" s="170"/>
       <c r="E7" s="110"/>
       <c r="F7" s="110"/>
       <c r="G7" s="110"/>
@@ -4309,12 +4528,12 @@
       <c r="P7" s="27"/>
       <c r="Q7" s="27"/>
       <c r="R7" s="27"/>
-      <c r="S7" s="41"/>
-      <c r="T7" s="40"/>
+      <c r="S7" s="218"/>
+      <c r="T7" s="231"/>
       <c r="U7" s="27"/>
       <c r="V7" s="27"/>
       <c r="W7" s="27"/>
-      <c r="X7" s="41"/>
+      <c r="X7" s="232"/>
       <c r="Y7" s="40"/>
       <c r="Z7" s="27"/>
       <c r="AA7" s="27"/>
@@ -4330,10 +4549,10 @@
       <c r="B8" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="179" t="s">
+      <c r="C8" s="169" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="180"/>
+      <c r="D8" s="170"/>
       <c r="E8" s="27"/>
       <c r="F8" s="27"/>
       <c r="G8" s="110"/>
@@ -4348,12 +4567,12 @@
       <c r="P8" s="27"/>
       <c r="Q8" s="27"/>
       <c r="R8" s="27"/>
-      <c r="S8" s="41"/>
-      <c r="T8" s="40"/>
+      <c r="S8" s="218"/>
+      <c r="T8" s="231"/>
       <c r="U8" s="27"/>
       <c r="V8" s="27"/>
       <c r="W8" s="27"/>
-      <c r="X8" s="41"/>
+      <c r="X8" s="232"/>
       <c r="Y8" s="40"/>
       <c r="Z8" s="27"/>
       <c r="AA8" s="27"/>
@@ -4369,10 +4588,10 @@
       <c r="B9" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="179" t="s">
+      <c r="C9" s="169" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="180"/>
+      <c r="D9" s="170"/>
       <c r="E9" s="27"/>
       <c r="F9" s="27"/>
       <c r="G9" s="110"/>
@@ -4387,12 +4606,12 @@
       <c r="P9" s="27"/>
       <c r="Q9" s="27"/>
       <c r="R9" s="27"/>
-      <c r="S9" s="41"/>
-      <c r="T9" s="40"/>
+      <c r="S9" s="218"/>
+      <c r="T9" s="231"/>
       <c r="U9" s="27"/>
       <c r="V9" s="27"/>
       <c r="W9" s="27"/>
-      <c r="X9" s="41"/>
+      <c r="X9" s="232"/>
       <c r="Y9" s="40"/>
       <c r="Z9" s="27"/>
       <c r="AA9" s="27"/>
@@ -4405,13 +4624,13 @@
       <c r="AH9" s="27"/>
     </row>
     <row r="10" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B10" s="167" t="s">
-        <v>70</v>
-      </c>
-      <c r="C10" s="181" t="s">
+      <c r="B10" s="183" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="193" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="182"/>
+      <c r="D10" s="194"/>
       <c r="E10" s="27"/>
       <c r="F10" s="27"/>
       <c r="G10" s="27"/>
@@ -4426,13 +4645,13 @@
       <c r="P10" s="125"/>
       <c r="Q10" s="125"/>
       <c r="R10" s="125"/>
-      <c r="S10" s="126"/>
-      <c r="T10" s="127"/>
+      <c r="S10" s="219"/>
+      <c r="T10" s="233"/>
       <c r="U10" s="125"/>
       <c r="V10" s="125"/>
       <c r="W10" s="125"/>
-      <c r="X10" s="126"/>
-      <c r="Y10" s="27"/>
+      <c r="X10" s="234"/>
+      <c r="Y10" s="40"/>
       <c r="Z10" s="27"/>
       <c r="AA10" s="27"/>
       <c r="AB10" s="27"/>
@@ -4444,11 +4663,11 @@
       <c r="AH10" s="27"/>
     </row>
     <row r="11" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B11" s="168"/>
-      <c r="C11" s="183" t="s">
+      <c r="B11" s="184"/>
+      <c r="C11" s="178" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="184"/>
+      <c r="D11" s="195"/>
       <c r="E11" s="27"/>
       <c r="F11" s="27"/>
       <c r="G11" s="27"/>
@@ -4463,13 +4682,13 @@
       <c r="P11" s="27"/>
       <c r="Q11" s="27"/>
       <c r="R11" s="27"/>
-      <c r="S11" s="41"/>
-      <c r="T11" s="40"/>
+      <c r="S11" s="218"/>
+      <c r="T11" s="231"/>
       <c r="U11" s="27"/>
       <c r="V11" s="27"/>
       <c r="W11" s="27"/>
-      <c r="X11" s="41"/>
-      <c r="Y11" s="27"/>
+      <c r="X11" s="232"/>
+      <c r="Y11" s="40"/>
       <c r="Z11" s="27"/>
       <c r="AA11" s="27"/>
       <c r="AB11" s="27"/>
@@ -4481,11 +4700,11 @@
       <c r="AH11" s="27"/>
     </row>
     <row r="12" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B12" s="168"/>
-      <c r="C12" s="185" t="s">
+      <c r="B12" s="184"/>
+      <c r="C12" s="196" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="186"/>
+      <c r="D12" s="197"/>
       <c r="E12" s="27"/>
       <c r="F12" s="27"/>
       <c r="G12" s="27"/>
@@ -4500,12 +4719,12 @@
       <c r="P12" s="119"/>
       <c r="Q12" s="119"/>
       <c r="R12" s="119"/>
-      <c r="S12" s="120"/>
-      <c r="T12" s="121"/>
+      <c r="S12" s="220"/>
+      <c r="T12" s="235"/>
       <c r="U12" s="119"/>
       <c r="V12" s="119"/>
       <c r="W12" s="119"/>
-      <c r="X12" s="120"/>
+      <c r="X12" s="236"/>
       <c r="Y12" s="40"/>
       <c r="Z12" s="27"/>
       <c r="AA12" s="27"/>
@@ -4518,11 +4737,11 @@
       <c r="AH12" s="27"/>
     </row>
     <row r="13" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B13" s="168"/>
-      <c r="C13" s="170" t="s">
+      <c r="B13" s="184"/>
+      <c r="C13" s="186" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="171"/>
+      <c r="D13" s="187"/>
       <c r="E13" s="27"/>
       <c r="F13" s="27"/>
       <c r="G13" s="27"/>
@@ -4531,18 +4750,18 @@
       <c r="J13" s="115"/>
       <c r="K13" s="113"/>
       <c r="L13" s="113"/>
-      <c r="M13" s="27"/>
-      <c r="N13" s="41"/>
-      <c r="O13" s="40"/>
-      <c r="P13" s="27"/>
-      <c r="Q13" s="27"/>
-      <c r="R13" s="27"/>
-      <c r="S13" s="41"/>
-      <c r="T13" s="40"/>
+      <c r="M13" s="113"/>
+      <c r="N13" s="114"/>
+      <c r="O13" s="115"/>
+      <c r="P13" s="113"/>
+      <c r="Q13" s="113"/>
+      <c r="R13" s="113"/>
+      <c r="S13" s="221"/>
+      <c r="T13" s="231"/>
       <c r="U13" s="27"/>
       <c r="V13" s="27"/>
       <c r="W13" s="27"/>
-      <c r="X13" s="41"/>
+      <c r="X13" s="232"/>
       <c r="Y13" s="40"/>
       <c r="Z13" s="27"/>
       <c r="AA13" s="27"/>
@@ -4555,11 +4774,11 @@
       <c r="AH13" s="27"/>
     </row>
     <row r="14" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B14" s="169"/>
-      <c r="C14" s="170" t="s">
+      <c r="B14" s="185"/>
+      <c r="C14" s="186" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="171"/>
+      <c r="D14" s="187"/>
       <c r="E14" s="27"/>
       <c r="G14" s="27"/>
       <c r="H14" s="116"/>
@@ -4567,18 +4786,18 @@
       <c r="J14" s="118"/>
       <c r="K14" s="116"/>
       <c r="L14" s="116"/>
-      <c r="M14" s="27"/>
-      <c r="N14" s="41"/>
-      <c r="O14" s="40"/>
-      <c r="P14" s="27"/>
-      <c r="Q14" s="27"/>
+      <c r="M14" s="116"/>
+      <c r="N14" s="117"/>
+      <c r="O14" s="118"/>
+      <c r="P14" s="116"/>
+      <c r="Q14" s="116"/>
       <c r="R14" s="27"/>
-      <c r="S14" s="41"/>
-      <c r="T14" s="40"/>
+      <c r="S14" s="218"/>
+      <c r="T14" s="231"/>
       <c r="U14" s="27"/>
       <c r="V14" s="27"/>
       <c r="W14" s="27"/>
-      <c r="X14" s="41"/>
+      <c r="X14" s="232"/>
       <c r="Y14" s="40"/>
       <c r="Z14" s="27"/>
       <c r="AA14" s="27"/>
@@ -4591,13 +4810,13 @@
       <c r="AH14" s="27"/>
     </row>
     <row r="15" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B15" s="190" t="s">
+      <c r="B15" s="201" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="192" t="s">
+      <c r="C15" s="203" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="193"/>
+      <c r="D15" s="204"/>
       <c r="E15" s="27"/>
       <c r="F15" s="27"/>
       <c r="G15" s="27"/>
@@ -4606,19 +4825,19 @@
       <c r="J15" s="40"/>
       <c r="K15" s="27"/>
       <c r="L15" s="27"/>
-      <c r="M15" s="113"/>
-      <c r="N15" s="114"/>
-      <c r="O15" s="113"/>
-      <c r="P15" s="113"/>
-      <c r="Q15" s="113"/>
-      <c r="R15" s="113"/>
-      <c r="S15" s="114"/>
-      <c r="T15" s="115"/>
+      <c r="M15" s="216"/>
+      <c r="N15" s="217"/>
+      <c r="O15" s="216"/>
+      <c r="P15" s="216"/>
+      <c r="Q15" s="216"/>
+      <c r="R15" s="216"/>
+      <c r="S15" s="222"/>
+      <c r="T15" s="237"/>
       <c r="U15" s="113"/>
       <c r="V15" s="113"/>
       <c r="W15" s="113"/>
-      <c r="X15" s="114"/>
-      <c r="Y15" s="27"/>
+      <c r="X15" s="238"/>
+      <c r="Y15" s="40"/>
       <c r="Z15" s="27"/>
       <c r="AA15" s="27"/>
       <c r="AB15" s="27"/>
@@ -4630,11 +4849,11 @@
       <c r="AH15" s="27"/>
     </row>
     <row r="16" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B16" s="191"/>
-      <c r="C16" s="172" t="s">
+      <c r="B16" s="202"/>
+      <c r="C16" s="167" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="173"/>
+      <c r="D16" s="168"/>
       <c r="E16" s="27"/>
       <c r="F16" s="27"/>
       <c r="G16" s="27"/>
@@ -4643,19 +4862,19 @@
       <c r="J16" s="40"/>
       <c r="K16" s="27"/>
       <c r="L16" s="27"/>
-      <c r="M16" s="116"/>
-      <c r="N16" s="117"/>
-      <c r="O16" s="116"/>
-      <c r="P16" s="116"/>
-      <c r="Q16" s="116"/>
+      <c r="M16" s="216"/>
+      <c r="N16" s="217"/>
+      <c r="O16" s="216"/>
+      <c r="P16" s="216"/>
+      <c r="Q16" s="216"/>
       <c r="R16" s="116"/>
-      <c r="S16" s="117"/>
-      <c r="T16" s="118"/>
+      <c r="S16" s="223"/>
+      <c r="T16" s="239"/>
       <c r="U16" s="116"/>
       <c r="V16" s="116"/>
       <c r="W16" s="116"/>
-      <c r="X16" s="117"/>
-      <c r="Y16" s="27"/>
+      <c r="X16" s="240"/>
+      <c r="Y16" s="40"/>
       <c r="Z16" s="27"/>
       <c r="AA16" s="27"/>
       <c r="AB16" s="27"/>
@@ -4670,10 +4889,10 @@
       <c r="B17" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="179" t="s">
+      <c r="C17" s="169" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="180"/>
+      <c r="D17" s="170"/>
       <c r="E17" s="27"/>
       <c r="F17" s="27"/>
       <c r="G17" s="27"/>
@@ -4688,12 +4907,12 @@
       <c r="P17" s="27"/>
       <c r="Q17" s="27"/>
       <c r="R17" s="27"/>
-      <c r="S17" s="41"/>
-      <c r="T17" s="40"/>
+      <c r="S17" s="218"/>
+      <c r="T17" s="231"/>
       <c r="U17" s="27"/>
       <c r="V17" s="27"/>
       <c r="W17" s="27"/>
-      <c r="X17" s="41"/>
+      <c r="X17" s="232"/>
       <c r="Y17" s="112"/>
       <c r="Z17" s="110"/>
       <c r="AA17" s="110"/>
@@ -4705,14 +4924,14 @@
       <c r="AG17" s="27"/>
       <c r="AH17" s="27"/>
     </row>
-    <row r="18" spans="2:34" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:34" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="172" t="s">
+      <c r="C18" s="167" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="173"/>
+      <c r="D18" s="168"/>
       <c r="E18" s="27"/>
       <c r="F18" s="27"/>
       <c r="G18" s="27"/>
@@ -4727,12 +4946,12 @@
       <c r="P18" s="27"/>
       <c r="Q18" s="27"/>
       <c r="R18" s="27"/>
-      <c r="S18" s="41"/>
-      <c r="T18" s="40"/>
-      <c r="U18" s="27"/>
-      <c r="V18" s="27"/>
-      <c r="W18" s="27"/>
-      <c r="X18" s="41"/>
+      <c r="S18" s="218"/>
+      <c r="T18" s="241"/>
+      <c r="U18" s="242"/>
+      <c r="V18" s="242"/>
+      <c r="W18" s="242"/>
+      <c r="X18" s="243"/>
       <c r="Y18" s="40"/>
       <c r="Z18" s="27"/>
       <c r="AA18" s="27"/>
@@ -4747,19 +4966,10 @@
     <row r="19" spans="2:34" x14ac:dyDescent="0.3">
       <c r="C19" s="28"/>
       <c r="D19" s="28"/>
+      <c r="V19" s="227"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E3:AH3"/>
-    <mergeCell ref="E4:AH4"/>
-    <mergeCell ref="T5:X5"/>
-    <mergeCell ref="Y5:AC5"/>
-    <mergeCell ref="E5:I5"/>
-    <mergeCell ref="J5:N5"/>
-    <mergeCell ref="O5:S5"/>
-    <mergeCell ref="AD5:AH5"/>
     <mergeCell ref="B10:B14"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C14:D14"/>
@@ -4776,6 +4986,16 @@
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E3:AH3"/>
+    <mergeCell ref="E4:AH4"/>
+    <mergeCell ref="T5:X5"/>
+    <mergeCell ref="Y5:AC5"/>
+    <mergeCell ref="E5:I5"/>
+    <mergeCell ref="J5:N5"/>
+    <mergeCell ref="O5:S5"/>
+    <mergeCell ref="AD5:AH5"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="C6:D12 C13:C14 C15:D18">
@@ -4798,7 +5018,7 @@
       <formula>NOT(ISERROR(SEARCH("김민수",C6)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C19:D19" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>$V$6:$V$16</formula1>
     </dataValidation>
@@ -4829,96 +5049,96 @@
   <sheetData>
     <row r="3" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="99" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="98" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="98" t="s">
+      <c r="D3" s="99" t="s">
         <v>51</v>
-      </c>
-      <c r="D3" s="99" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" s="205" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" s="102" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D4" s="96" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" s="205"/>
       <c r="C5" s="102" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D5" s="104" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" s="206"/>
       <c r="C6" s="103" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="95" t="s">
         <v>57</v>
-      </c>
-      <c r="D6" s="95" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B7" s="207" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C7" s="100" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D7" s="105" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8" s="208"/>
       <c r="C8" s="101" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D8" s="104" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B9" s="208"/>
       <c r="C9" s="101" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D9" s="104" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B10" s="208"/>
       <c r="C10" s="210" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D10" s="104" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B11" s="208"/>
       <c r="C11" s="211"/>
       <c r="D11" s="104" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B12" s="209"/>
       <c r="C12" s="97" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D12" s="95" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ECR & lambda & Dash integration
</commit_message>
<xml_diff>
--- a/Final_pjt2/WBS.xlsx
+++ b/Final_pjt2/WBS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Genia\Final_pjt2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE2F77E-F064-4B3A-8743-552AB5CEB3B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1CCBAD-7FEC-4C57-BCBC-D01DCB0F762F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15030" yWindow="645" windowWidth="23370" windowHeight="20070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15030" yWindow="645" windowWidth="23370" windowHeight="20070" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WBS" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="224">
   <si>
     <t>테스트</t>
   </si>
@@ -450,10 +450,6 @@
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>USER_M</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
     <t>name</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
@@ -903,6 +899,18 @@
   </si>
   <si>
     <t>Auto Increase Number</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>ind</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>USER_LMP</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>숫자 Index</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -910,11 +918,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="176" formatCode="yyyy\/mm\/dd\(aaa\)"/>
     <numFmt numFmtId="177" formatCode="0.0%"/>
     <numFmt numFmtId="178" formatCode="0.0_ "/>
     <numFmt numFmtId="179" formatCode="0_ "/>
+    <numFmt numFmtId="182" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -2438,7 +2447,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="300">
+  <cellXfs count="291">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2940,6 +2949,75 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="97" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="98" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="99" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="99" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="99" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="99" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="99" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="34" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="91" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="91" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="91" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="91" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="93" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="94" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="94" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="95" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="100" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="84" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3066,58 +3144,19 @@
     <xf numFmtId="176" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3135,6 +3174,12 @@
     <xf numFmtId="0" fontId="8" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3156,6 +3201,9 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="16" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3174,18 +3222,60 @@
     <xf numFmtId="0" fontId="5" fillId="12" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="15" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="15" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="17" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3222,121 +3312,13 @@
     <xf numFmtId="0" fontId="12" fillId="26" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="182" fontId="8" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="97" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="98" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="99" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="99" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="99" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="99" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="99" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="99" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="34" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="91" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="91" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="91" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="91" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="93" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="94" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="94" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="95" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="100" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4020,7 +4002,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="75" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="75" workbookViewId="0">
       <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
@@ -4056,12 +4038,12 @@
     </row>
     <row r="2" spans="1:13" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="53"/>
-      <c r="B2" s="167" t="s">
+      <c r="B2" s="190" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="168"/>
-      <c r="D2" s="168"/>
-      <c r="E2" s="168"/>
+      <c r="C2" s="191"/>
+      <c r="D2" s="191"/>
+      <c r="E2" s="191"/>
       <c r="F2" s="100"/>
       <c r="G2" s="100"/>
       <c r="H2" s="100"/>
@@ -4070,7 +4052,7 @@
       </c>
       <c r="J2" s="101">
         <f ca="1">TODAY()</f>
-        <v>45286</v>
+        <v>45287</v>
       </c>
       <c r="K2" s="102" t="s">
         <v>31</v>
@@ -4083,44 +4065,44 @@
     </row>
     <row r="3" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="81"/>
-      <c r="B3" s="179" t="s">
+      <c r="B3" s="202" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="181" t="s">
+      <c r="C3" s="204" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="183" t="s">
+      <c r="D3" s="206" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="185" t="s">
+      <c r="E3" s="208" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="186"/>
-      <c r="G3" s="186"/>
-      <c r="H3" s="186"/>
-      <c r="I3" s="187"/>
-      <c r="J3" s="198" t="s">
+      <c r="F3" s="209"/>
+      <c r="G3" s="209"/>
+      <c r="H3" s="209"/>
+      <c r="I3" s="210"/>
+      <c r="J3" s="221" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="172" t="s">
+      <c r="K3" s="195" t="s">
         <v>27</v>
       </c>
-      <c r="L3" s="173"/>
+      <c r="L3" s="196"/>
       <c r="M3" s="30"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="81"/>
-      <c r="B4" s="180"/>
-      <c r="C4" s="182"/>
-      <c r="D4" s="184"/>
-      <c r="E4" s="188"/>
-      <c r="F4" s="189"/>
-      <c r="G4" s="189"/>
-      <c r="H4" s="189"/>
-      <c r="I4" s="190"/>
-      <c r="J4" s="199"/>
-      <c r="K4" s="174"/>
-      <c r="L4" s="175"/>
+      <c r="B4" s="203"/>
+      <c r="C4" s="205"/>
+      <c r="D4" s="207"/>
+      <c r="E4" s="211"/>
+      <c r="F4" s="212"/>
+      <c r="G4" s="212"/>
+      <c r="H4" s="212"/>
+      <c r="I4" s="213"/>
+      <c r="J4" s="222"/>
+      <c r="K4" s="197"/>
+      <c r="L4" s="198"/>
     </row>
     <row r="5" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="81"/>
@@ -4144,7 +4126,7 @@
       <c r="I5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="200"/>
+      <c r="J5" s="223"/>
       <c r="K5" s="78" t="s">
         <v>6</v>
       </c>
@@ -4154,10 +4136,10 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="81"/>
-      <c r="B6" s="193" t="s">
+      <c r="B6" s="216" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="194"/>
+      <c r="C6" s="217"/>
       <c r="D6" s="16"/>
       <c r="E6" s="17" t="str">
         <f>CONCATENATE(NETWORKDAYS(F6,G6),"일")</f>
@@ -4188,15 +4170,15 @@
       </c>
       <c r="L6" s="31">
         <f t="shared" ref="L6:L28" ca="1" si="0">IF(G6-$J$2&lt;=0,0,G6-$J$2)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="81"/>
-      <c r="B7" s="201" t="s">
+      <c r="B7" s="224" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="202"/>
+      <c r="C7" s="225"/>
       <c r="D7" s="13"/>
       <c r="E7" s="13" t="str">
         <f>CONCATENATE(NETWORKDAYS(F7,G7),"일")</f>
@@ -4226,13 +4208,13 @@
       </c>
       <c r="L7" s="32">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M7" s="36"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="81"/>
-      <c r="B8" s="203" t="s">
+      <c r="B8" s="226" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="52" t="s">
@@ -4267,12 +4249,12 @@
       </c>
       <c r="L8" s="33">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="81"/>
-      <c r="B9" s="204"/>
+      <c r="B9" s="227"/>
       <c r="C9" s="3" t="s">
         <v>21</v>
       </c>
@@ -4310,7 +4292,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="81"/>
-      <c r="B10" s="204"/>
+      <c r="B10" s="227"/>
       <c r="C10" s="3" t="s">
         <v>35</v>
       </c>
@@ -4348,7 +4330,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="81"/>
-      <c r="B11" s="204"/>
+      <c r="B11" s="227"/>
       <c r="C11" s="3" t="s">
         <v>41</v>
       </c>
@@ -4386,7 +4368,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="81"/>
-      <c r="B12" s="204"/>
+      <c r="B12" s="227"/>
       <c r="C12" s="3" t="s">
         <v>42</v>
       </c>
@@ -4424,7 +4406,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="81"/>
-      <c r="B13" s="204"/>
+      <c r="B13" s="227"/>
       <c r="C13" s="88" t="s">
         <v>45</v>
       </c>
@@ -4462,7 +4444,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="81"/>
-      <c r="B14" s="204"/>
+      <c r="B14" s="227"/>
       <c r="C14" s="3" t="s">
         <v>48</v>
       </c>
@@ -4479,7 +4461,7 @@
       <c r="G14" s="20">
         <v>45258</v>
       </c>
-      <c r="H14" s="206" t="s">
+      <c r="H14" s="229" t="s">
         <v>2</v>
       </c>
       <c r="I14" s="85">
@@ -4500,7 +4482,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="81"/>
-      <c r="B15" s="204"/>
+      <c r="B15" s="227"/>
       <c r="C15" s="88" t="s">
         <v>67</v>
       </c>
@@ -4517,7 +4499,7 @@
       <c r="G15" s="20">
         <v>45258</v>
       </c>
-      <c r="H15" s="207"/>
+      <c r="H15" s="230"/>
       <c r="I15" s="85">
         <v>1</v>
       </c>
@@ -4536,7 +4518,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="81"/>
-      <c r="B16" s="205"/>
+      <c r="B16" s="228"/>
       <c r="C16" s="51" t="s">
         <v>68</v>
       </c>
@@ -4553,7 +4535,7 @@
       <c r="G16" s="20">
         <v>45258</v>
       </c>
-      <c r="H16" s="208"/>
+      <c r="H16" s="231"/>
       <c r="I16" s="85">
         <v>0.9</v>
       </c>
@@ -4572,10 +4554,10 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="81"/>
-      <c r="B17" s="201" t="s">
+      <c r="B17" s="224" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="202"/>
+      <c r="C17" s="225"/>
       <c r="D17" s="21"/>
       <c r="E17" s="21" t="str">
         <f>CONCATENATE(NETWORKDAYS(F17,G17),"일")</f>
@@ -4608,10 +4590,10 @@
     </row>
     <row r="18" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="81"/>
-      <c r="B18" s="176" t="s">
+      <c r="B18" s="199" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="195" t="s">
+      <c r="C18" s="218" t="s">
         <v>74</v>
       </c>
       <c r="D18" s="50" t="s">
@@ -4648,8 +4630,8 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="81"/>
-      <c r="B19" s="177"/>
-      <c r="C19" s="196"/>
+      <c r="B19" s="200"/>
+      <c r="C19" s="219"/>
       <c r="D19" s="50" t="s">
         <v>11</v>
       </c>
@@ -4684,8 +4666,8 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="81"/>
-      <c r="B20" s="177"/>
-      <c r="C20" s="196"/>
+      <c r="B20" s="200"/>
+      <c r="C20" s="219"/>
       <c r="D20" s="47" t="s">
         <v>11</v>
       </c>
@@ -4720,8 +4702,8 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="81"/>
-      <c r="B21" s="177"/>
-      <c r="C21" s="197"/>
+      <c r="B21" s="200"/>
+      <c r="C21" s="220"/>
       <c r="D21" s="47" t="s">
         <v>11</v>
       </c>
@@ -4756,7 +4738,7 @@
     </row>
     <row r="22" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A22" s="81"/>
-      <c r="B22" s="177"/>
+      <c r="B22" s="200"/>
       <c r="C22" s="122" t="s">
         <v>75</v>
       </c>
@@ -4794,8 +4776,8 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="81"/>
-      <c r="B23" s="177"/>
-      <c r="C23" s="191" t="s">
+      <c r="B23" s="200"/>
+      <c r="C23" s="214" t="s">
         <v>46</v>
       </c>
       <c r="D23" s="47" t="s">
@@ -4832,8 +4814,8 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="81"/>
-      <c r="B24" s="177"/>
-      <c r="C24" s="192"/>
+      <c r="B24" s="200"/>
+      <c r="C24" s="215"/>
       <c r="D24" s="6" t="s">
         <v>11</v>
       </c>
@@ -4868,7 +4850,7 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="81"/>
-      <c r="B25" s="178"/>
+      <c r="B25" s="201"/>
       <c r="C25" s="51" t="s">
         <v>77</v>
       </c>
@@ -5016,12 +4998,12 @@
       </c>
       <c r="L28" s="34">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="81"/>
-      <c r="B29" s="169" t="s">
+      <c r="B29" s="192" t="s">
         <v>25</v>
       </c>
       <c r="C29" s="48" t="s">
@@ -5056,12 +5038,12 @@
       </c>
       <c r="L29" s="37">
         <f ca="1">IF(G30-$J$2&lt;=0,0,G30-$J$2)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="81"/>
-      <c r="B30" s="170"/>
+      <c r="B30" s="193"/>
       <c r="C30" s="49" t="s">
         <v>23</v>
       </c>
@@ -5094,12 +5076,12 @@
       </c>
       <c r="L30" s="33">
         <f ca="1">IF(G31-$J$2&lt;=0,0,G31-$J$2)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="53"/>
-      <c r="B31" s="171"/>
+      <c r="B31" s="194"/>
       <c r="C31" s="68" t="s">
         <v>7</v>
       </c>
@@ -5122,7 +5104,7 @@
       <c r="I31" s="73">
         <v>0</v>
       </c>
-      <c r="J31" s="299">
+      <c r="J31" s="189">
         <f>$J$28/COUNT($I$29:$I$31)</f>
         <v>3.3333333333333333E-2</v>
       </c>
@@ -5132,11 +5114,11 @@
       </c>
       <c r="L31" s="75">
         <f ca="1">IF(G31-$J$2&lt;=0,0,G31-$J$2)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="J32" s="298"/>
+      <c r="J32" s="188"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -5232,140 +5214,140 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B3" s="232" t="s">
+      <c r="B3" s="244" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="234" t="s">
+      <c r="C3" s="246" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="234"/>
-      <c r="E3" s="213" t="s">
+      <c r="D3" s="246"/>
+      <c r="E3" s="260" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="214"/>
-      <c r="G3" s="214"/>
-      <c r="H3" s="214"/>
-      <c r="I3" s="214"/>
-      <c r="J3" s="214"/>
-      <c r="K3" s="214"/>
-      <c r="L3" s="214"/>
-      <c r="M3" s="214"/>
-      <c r="N3" s="214"/>
-      <c r="O3" s="214"/>
-      <c r="P3" s="214"/>
-      <c r="Q3" s="214"/>
-      <c r="R3" s="214"/>
-      <c r="S3" s="214"/>
-      <c r="T3" s="214"/>
-      <c r="U3" s="214"/>
-      <c r="V3" s="214"/>
-      <c r="W3" s="214"/>
-      <c r="X3" s="214"/>
-      <c r="Y3" s="214"/>
-      <c r="Z3" s="214"/>
-      <c r="AA3" s="214"/>
-      <c r="AB3" s="214"/>
-      <c r="AC3" s="214"/>
-      <c r="AD3" s="214"/>
-      <c r="AE3" s="214"/>
-      <c r="AF3" s="214"/>
-      <c r="AG3" s="214"/>
-      <c r="AH3" s="215"/>
+      <c r="F3" s="261"/>
+      <c r="G3" s="261"/>
+      <c r="H3" s="261"/>
+      <c r="I3" s="261"/>
+      <c r="J3" s="261"/>
+      <c r="K3" s="261"/>
+      <c r="L3" s="261"/>
+      <c r="M3" s="261"/>
+      <c r="N3" s="261"/>
+      <c r="O3" s="261"/>
+      <c r="P3" s="261"/>
+      <c r="Q3" s="261"/>
+      <c r="R3" s="261"/>
+      <c r="S3" s="261"/>
+      <c r="T3" s="261"/>
+      <c r="U3" s="261"/>
+      <c r="V3" s="261"/>
+      <c r="W3" s="261"/>
+      <c r="X3" s="261"/>
+      <c r="Y3" s="261"/>
+      <c r="Z3" s="261"/>
+      <c r="AA3" s="261"/>
+      <c r="AB3" s="261"/>
+      <c r="AC3" s="261"/>
+      <c r="AD3" s="261"/>
+      <c r="AE3" s="261"/>
+      <c r="AF3" s="261"/>
+      <c r="AG3" s="261"/>
+      <c r="AH3" s="262"/>
     </row>
     <row r="4" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B4" s="233"/>
-      <c r="C4" s="235"/>
-      <c r="D4" s="236"/>
-      <c r="E4" s="216" t="s">
+      <c r="B4" s="245"/>
+      <c r="C4" s="247"/>
+      <c r="D4" s="248"/>
+      <c r="E4" s="263" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="217"/>
-      <c r="G4" s="217"/>
-      <c r="H4" s="217"/>
-      <c r="I4" s="217"/>
-      <c r="J4" s="217"/>
-      <c r="K4" s="217"/>
-      <c r="L4" s="217"/>
-      <c r="M4" s="217"/>
-      <c r="N4" s="217"/>
-      <c r="O4" s="217"/>
-      <c r="P4" s="217"/>
-      <c r="Q4" s="217"/>
-      <c r="R4" s="217"/>
-      <c r="S4" s="217"/>
-      <c r="T4" s="217"/>
-      <c r="U4" s="217"/>
-      <c r="V4" s="217"/>
-      <c r="W4" s="217"/>
-      <c r="X4" s="217"/>
-      <c r="Y4" s="217"/>
-      <c r="Z4" s="217"/>
-      <c r="AA4" s="217"/>
-      <c r="AB4" s="217"/>
-      <c r="AC4" s="217"/>
-      <c r="AD4" s="217"/>
-      <c r="AE4" s="217"/>
-      <c r="AF4" s="217"/>
-      <c r="AG4" s="217"/>
-      <c r="AH4" s="218"/>
+      <c r="F4" s="264"/>
+      <c r="G4" s="264"/>
+      <c r="H4" s="264"/>
+      <c r="I4" s="264"/>
+      <c r="J4" s="264"/>
+      <c r="K4" s="264"/>
+      <c r="L4" s="264"/>
+      <c r="M4" s="264"/>
+      <c r="N4" s="264"/>
+      <c r="O4" s="264"/>
+      <c r="P4" s="264"/>
+      <c r="Q4" s="264"/>
+      <c r="R4" s="264"/>
+      <c r="S4" s="264"/>
+      <c r="T4" s="264"/>
+      <c r="U4" s="264"/>
+      <c r="V4" s="264"/>
+      <c r="W4" s="264"/>
+      <c r="X4" s="264"/>
+      <c r="Y4" s="264"/>
+      <c r="Z4" s="264"/>
+      <c r="AA4" s="264"/>
+      <c r="AB4" s="264"/>
+      <c r="AC4" s="264"/>
+      <c r="AD4" s="264"/>
+      <c r="AE4" s="264"/>
+      <c r="AF4" s="264"/>
+      <c r="AG4" s="264"/>
+      <c r="AH4" s="265"/>
     </row>
     <row r="5" spans="2:34" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="242" t="s">
+      <c r="B5" s="255" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="243"/>
-      <c r="D5" s="244"/>
-      <c r="E5" s="222">
+      <c r="C5" s="256"/>
+      <c r="D5" s="257"/>
+      <c r="E5" s="251">
         <v>1</v>
       </c>
-      <c r="F5" s="223"/>
-      <c r="G5" s="223"/>
-      <c r="H5" s="223"/>
-      <c r="I5" s="224"/>
-      <c r="J5" s="225">
+      <c r="F5" s="269"/>
+      <c r="G5" s="269"/>
+      <c r="H5" s="269"/>
+      <c r="I5" s="270"/>
+      <c r="J5" s="271">
         <v>2</v>
       </c>
-      <c r="K5" s="217"/>
-      <c r="L5" s="217"/>
-      <c r="M5" s="217"/>
-      <c r="N5" s="218"/>
-      <c r="O5" s="226">
+      <c r="K5" s="264"/>
+      <c r="L5" s="264"/>
+      <c r="M5" s="264"/>
+      <c r="N5" s="265"/>
+      <c r="O5" s="272">
         <v>3</v>
       </c>
-      <c r="P5" s="217"/>
-      <c r="Q5" s="217"/>
-      <c r="R5" s="217"/>
-      <c r="S5" s="218"/>
-      <c r="T5" s="219">
+      <c r="P5" s="264"/>
+      <c r="Q5" s="264"/>
+      <c r="R5" s="264"/>
+      <c r="S5" s="265"/>
+      <c r="T5" s="266">
         <v>4</v>
       </c>
-      <c r="U5" s="220"/>
-      <c r="V5" s="220"/>
-      <c r="W5" s="220"/>
-      <c r="X5" s="221"/>
-      <c r="Y5" s="219">
+      <c r="U5" s="267"/>
+      <c r="V5" s="267"/>
+      <c r="W5" s="267"/>
+      <c r="X5" s="268"/>
+      <c r="Y5" s="266">
         <v>5</v>
       </c>
-      <c r="Z5" s="220"/>
-      <c r="AA5" s="220"/>
-      <c r="AB5" s="220"/>
-      <c r="AC5" s="221"/>
-      <c r="AD5" s="287">
+      <c r="Z5" s="267"/>
+      <c r="AA5" s="267"/>
+      <c r="AB5" s="267"/>
+      <c r="AC5" s="268"/>
+      <c r="AD5" s="273">
         <v>6</v>
       </c>
-      <c r="AE5" s="288"/>
-      <c r="AF5" s="288"/>
-      <c r="AG5" s="288"/>
-      <c r="AH5" s="289"/>
+      <c r="AE5" s="274"/>
+      <c r="AF5" s="274"/>
+      <c r="AG5" s="274"/>
+      <c r="AH5" s="275"/>
     </row>
     <row r="6" spans="2:34" x14ac:dyDescent="0.3">
       <c r="B6" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="211" t="s">
+      <c r="C6" s="232" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="212"/>
+      <c r="D6" s="233"/>
       <c r="E6" s="104"/>
       <c r="F6" s="104"/>
       <c r="G6" s="104"/>
@@ -5386,7 +5368,7 @@
       <c r="V6" s="27"/>
       <c r="W6" s="27"/>
       <c r="X6" s="123"/>
-      <c r="Y6" s="275"/>
+      <c r="Y6" s="174"/>
       <c r="Z6" s="27"/>
       <c r="AA6" s="27"/>
       <c r="AB6" s="27"/>
@@ -5401,10 +5383,10 @@
       <c r="B7" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="211" t="s">
+      <c r="C7" s="232" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="212"/>
+      <c r="D7" s="233"/>
       <c r="E7" s="104"/>
       <c r="F7" s="104"/>
       <c r="G7" s="104"/>
@@ -5425,7 +5407,7 @@
       <c r="V7" s="27"/>
       <c r="W7" s="27"/>
       <c r="X7" s="123"/>
-      <c r="Y7" s="275"/>
+      <c r="Y7" s="174"/>
       <c r="Z7" s="27"/>
       <c r="AA7" s="27"/>
       <c r="AB7" s="27"/>
@@ -5440,10 +5422,10 @@
       <c r="B8" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="211" t="s">
+      <c r="C8" s="232" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="212"/>
+      <c r="D8" s="233"/>
       <c r="E8" s="27"/>
       <c r="F8" s="27"/>
       <c r="G8" s="104"/>
@@ -5464,7 +5446,7 @@
       <c r="V8" s="27"/>
       <c r="W8" s="27"/>
       <c r="X8" s="123"/>
-      <c r="Y8" s="275"/>
+      <c r="Y8" s="174"/>
       <c r="Z8" s="27"/>
       <c r="AA8" s="27"/>
       <c r="AB8" s="27"/>
@@ -5479,10 +5461,10 @@
       <c r="B9" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="211" t="s">
+      <c r="C9" s="232" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="212"/>
+      <c r="D9" s="233"/>
       <c r="E9" s="27"/>
       <c r="F9" s="27"/>
       <c r="G9" s="104"/>
@@ -5503,7 +5485,7 @@
       <c r="V9" s="27"/>
       <c r="W9" s="27"/>
       <c r="X9" s="123"/>
-      <c r="Y9" s="275"/>
+      <c r="Y9" s="174"/>
       <c r="Z9" s="27"/>
       <c r="AA9" s="27"/>
       <c r="AB9" s="27"/>
@@ -5515,13 +5497,13 @@
       <c r="AH9" s="132"/>
     </row>
     <row r="10" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B10" s="227" t="s">
+      <c r="B10" s="237" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="237" t="s">
+      <c r="C10" s="249" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="238"/>
+      <c r="D10" s="250"/>
       <c r="E10" s="27"/>
       <c r="F10" s="27"/>
       <c r="G10" s="27"/>
@@ -5542,23 +5524,23 @@
       <c r="V10" s="119"/>
       <c r="W10" s="119"/>
       <c r="X10" s="124"/>
-      <c r="Y10" s="280"/>
+      <c r="Y10" s="175"/>
       <c r="Z10" s="119"/>
       <c r="AA10" s="119"/>
       <c r="AB10" s="119"/>
       <c r="AC10" s="124"/>
-      <c r="AD10" s="290"/>
+      <c r="AD10" s="180"/>
       <c r="AE10" s="119"/>
       <c r="AF10" s="119"/>
       <c r="AG10" s="27"/>
       <c r="AH10" s="132"/>
     </row>
     <row r="11" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B11" s="228"/>
-      <c r="C11" s="222" t="s">
+      <c r="B11" s="238"/>
+      <c r="C11" s="251" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="239"/>
+      <c r="D11" s="252"/>
       <c r="E11" s="27"/>
       <c r="F11" s="27"/>
       <c r="G11" s="27"/>
@@ -5579,7 +5561,7 @@
       <c r="V11" s="27"/>
       <c r="W11" s="27"/>
       <c r="X11" s="123"/>
-      <c r="Y11" s="275"/>
+      <c r="Y11" s="174"/>
       <c r="Z11" s="27"/>
       <c r="AA11" s="27"/>
       <c r="AB11" s="27"/>
@@ -5591,11 +5573,11 @@
       <c r="AH11" s="132"/>
     </row>
     <row r="12" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B12" s="228"/>
-      <c r="C12" s="240" t="s">
+      <c r="B12" s="238"/>
+      <c r="C12" s="253" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="241"/>
+      <c r="D12" s="254"/>
       <c r="E12" s="27"/>
       <c r="F12" s="27"/>
       <c r="G12" s="27"/>
@@ -5616,7 +5598,7 @@
       <c r="V12" s="113"/>
       <c r="W12" s="113"/>
       <c r="X12" s="125"/>
-      <c r="Y12" s="275"/>
+      <c r="Y12" s="174"/>
       <c r="Z12" s="27"/>
       <c r="AA12" s="27"/>
       <c r="AB12" s="27"/>
@@ -5628,11 +5610,11 @@
       <c r="AH12" s="132"/>
     </row>
     <row r="13" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B13" s="228"/>
-      <c r="C13" s="230" t="s">
+      <c r="B13" s="238"/>
+      <c r="C13" s="240" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="231"/>
+      <c r="D13" s="241"/>
       <c r="E13" s="27"/>
       <c r="F13" s="27"/>
       <c r="G13" s="27"/>
@@ -5653,7 +5635,7 @@
       <c r="V13" s="27"/>
       <c r="W13" s="27"/>
       <c r="X13" s="123"/>
-      <c r="Y13" s="275"/>
+      <c r="Y13" s="174"/>
       <c r="Z13" s="27"/>
       <c r="AA13" s="27"/>
       <c r="AB13" s="27"/>
@@ -5665,11 +5647,11 @@
       <c r="AH13" s="132"/>
     </row>
     <row r="14" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B14" s="229"/>
-      <c r="C14" s="230" t="s">
+      <c r="B14" s="239"/>
+      <c r="C14" s="240" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="231"/>
+      <c r="D14" s="241"/>
       <c r="E14" s="27"/>
       <c r="G14" s="27"/>
       <c r="H14" s="110"/>
@@ -5689,7 +5671,7 @@
       <c r="V14" s="27"/>
       <c r="W14" s="27"/>
       <c r="X14" s="123"/>
-      <c r="Y14" s="275"/>
+      <c r="Y14" s="174"/>
       <c r="Z14" s="27"/>
       <c r="AA14" s="27"/>
       <c r="AB14" s="27"/>
@@ -5701,13 +5683,13 @@
       <c r="AH14" s="132"/>
     </row>
     <row r="15" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B15" s="245" t="s">
+      <c r="B15" s="234" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="247" t="s">
+      <c r="C15" s="258" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="248"/>
+      <c r="D15" s="259"/>
       <c r="E15" s="27"/>
       <c r="F15" s="27"/>
       <c r="G15" s="27"/>
@@ -5728,23 +5710,23 @@
       <c r="V15" s="107"/>
       <c r="W15" s="107"/>
       <c r="X15" s="126"/>
-      <c r="Y15" s="282"/>
+      <c r="Y15" s="176"/>
       <c r="Z15" s="107"/>
       <c r="AA15" s="107"/>
       <c r="AB15" s="107"/>
       <c r="AC15" s="126"/>
-      <c r="AD15" s="291"/>
+      <c r="AD15" s="181"/>
       <c r="AE15" s="107"/>
       <c r="AF15" s="107"/>
       <c r="AG15" s="27"/>
       <c r="AH15" s="132"/>
     </row>
     <row r="16" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B16" s="281"/>
-      <c r="C16" s="209" t="s">
+      <c r="B16" s="235"/>
+      <c r="C16" s="242" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="210"/>
+      <c r="D16" s="243"/>
       <c r="E16" s="27"/>
       <c r="F16" s="27"/>
       <c r="G16" s="27"/>
@@ -5765,23 +5747,23 @@
       <c r="V16" s="110"/>
       <c r="W16" s="110"/>
       <c r="X16" s="127"/>
-      <c r="Y16" s="283"/>
+      <c r="Y16" s="177"/>
       <c r="Z16" s="110"/>
       <c r="AA16" s="110"/>
       <c r="AB16" s="110"/>
       <c r="AC16" s="127"/>
-      <c r="AD16" s="292"/>
+      <c r="AD16" s="182"/>
       <c r="AE16" s="110"/>
       <c r="AF16" s="110"/>
       <c r="AG16" s="27"/>
       <c r="AH16" s="132"/>
     </row>
     <row r="17" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B17" s="246"/>
-      <c r="C17" s="211" t="s">
+      <c r="B17" s="236"/>
+      <c r="C17" s="232" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="212"/>
+      <c r="D17" s="233"/>
       <c r="E17" s="27"/>
       <c r="F17" s="27"/>
       <c r="G17" s="27"/>
@@ -5795,19 +5777,19 @@
       <c r="O17" s="40"/>
       <c r="P17" s="27"/>
       <c r="Q17" s="27"/>
-      <c r="R17" s="277"/>
-      <c r="S17" s="279"/>
-      <c r="T17" s="276"/>
-      <c r="U17" s="277"/>
-      <c r="V17" s="277"/>
-      <c r="W17" s="277"/>
-      <c r="X17" s="285"/>
-      <c r="Y17" s="284"/>
+      <c r="R17" s="27"/>
+      <c r="S17" s="41"/>
+      <c r="T17" s="40"/>
+      <c r="U17" s="27"/>
+      <c r="V17" s="27"/>
+      <c r="W17" s="27"/>
+      <c r="X17" s="123"/>
+      <c r="Y17" s="178"/>
       <c r="Z17" s="113"/>
       <c r="AA17" s="113"/>
       <c r="AB17" s="113"/>
       <c r="AC17" s="125"/>
-      <c r="AD17" s="293"/>
+      <c r="AD17" s="183"/>
       <c r="AE17" s="113"/>
       <c r="AF17" s="113"/>
       <c r="AG17" s="27"/>
@@ -5817,10 +5799,10 @@
       <c r="B18" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="211" t="s">
+      <c r="C18" s="232" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="212"/>
+      <c r="D18" s="233"/>
       <c r="E18" s="27"/>
       <c r="F18" s="27"/>
       <c r="G18" s="27"/>
@@ -5841,11 +5823,11 @@
       <c r="V18" s="27"/>
       <c r="W18" s="27"/>
       <c r="X18" s="123"/>
-      <c r="Y18" s="278"/>
-      <c r="Z18" s="277"/>
-      <c r="AA18" s="277"/>
-      <c r="AB18" s="277"/>
-      <c r="AC18" s="286"/>
+      <c r="Y18" s="174"/>
+      <c r="Z18" s="27"/>
+      <c r="AA18" s="27"/>
+      <c r="AB18" s="27"/>
+      <c r="AC18" s="179"/>
       <c r="AD18" s="133"/>
       <c r="AE18" s="104"/>
       <c r="AF18" s="104"/>
@@ -5856,10 +5838,10 @@
       <c r="B19" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="209" t="s">
+      <c r="C19" s="242" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="210"/>
+      <c r="D19" s="243"/>
       <c r="E19" s="27"/>
       <c r="F19" s="27"/>
       <c r="G19" s="27"/>
@@ -5880,16 +5862,16 @@
       <c r="V19" s="27"/>
       <c r="W19" s="27"/>
       <c r="X19" s="123"/>
-      <c r="Y19" s="275"/>
+      <c r="Y19" s="174"/>
       <c r="Z19" s="27"/>
       <c r="AA19" s="27"/>
       <c r="AB19" s="27"/>
       <c r="AC19" s="123"/>
-      <c r="AD19" s="294"/>
-      <c r="AE19" s="295"/>
-      <c r="AF19" s="295"/>
-      <c r="AG19" s="296"/>
-      <c r="AH19" s="297"/>
+      <c r="AD19" s="184"/>
+      <c r="AE19" s="185"/>
+      <c r="AF19" s="185"/>
+      <c r="AG19" s="186"/>
+      <c r="AH19" s="187"/>
     </row>
     <row r="20" spans="2:34" x14ac:dyDescent="0.3">
       <c r="C20" s="28"/>
@@ -5897,11 +5879,14 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="B10:B14"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E3:AH3"/>
+    <mergeCell ref="E4:AH4"/>
+    <mergeCell ref="T5:X5"/>
+    <mergeCell ref="Y5:AC5"/>
+    <mergeCell ref="E5:I5"/>
+    <mergeCell ref="J5:N5"/>
+    <mergeCell ref="O5:S5"/>
+    <mergeCell ref="AD5:AH5"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:D4"/>
@@ -5916,17 +5901,14 @@
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E3:AH3"/>
-    <mergeCell ref="E4:AH4"/>
-    <mergeCell ref="T5:X5"/>
-    <mergeCell ref="Y5:AC5"/>
-    <mergeCell ref="E5:I5"/>
-    <mergeCell ref="J5:N5"/>
-    <mergeCell ref="O5:S5"/>
-    <mergeCell ref="AD5:AH5"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
-  <conditionalFormatting sqref="C6:D12 C13:C14 C15:D16 C18:D19 C17">
+  <conditionalFormatting sqref="C6:D12 C13:C14 C15:D16 C17 C18:D19">
     <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="공통">
       <formula>NOT(ISERROR(SEARCH("공통",C6)))</formula>
     </cfRule>
@@ -5987,7 +5969,7 @@
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B4" s="249" t="s">
+      <c r="B4" s="276" t="s">
         <v>52</v>
       </c>
       <c r="C4" s="96" t="s">
@@ -5998,7 +5980,7 @@
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B5" s="249"/>
+      <c r="B5" s="276"/>
       <c r="C5" s="96" t="s">
         <v>53</v>
       </c>
@@ -6007,7 +5989,7 @@
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="250"/>
+      <c r="B6" s="277"/>
       <c r="C6" s="97" t="s">
         <v>56</v>
       </c>
@@ -6016,7 +5998,7 @@
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="251" t="s">
+      <c r="B7" s="278" t="s">
         <v>54</v>
       </c>
       <c r="C7" s="94" t="s">
@@ -6027,7 +6009,7 @@
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B8" s="252"/>
+      <c r="B8" s="279"/>
       <c r="C8" s="95" t="s">
         <v>59</v>
       </c>
@@ -6036,7 +6018,7 @@
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="252"/>
+      <c r="B9" s="279"/>
       <c r="C9" s="95" t="s">
         <v>66</v>
       </c>
@@ -6045,8 +6027,8 @@
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B10" s="252"/>
-      <c r="C10" s="254" t="s">
+      <c r="B10" s="279"/>
+      <c r="C10" s="281" t="s">
         <v>60</v>
       </c>
       <c r="D10" s="98" t="s">
@@ -6054,14 +6036,14 @@
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B11" s="252"/>
-      <c r="C11" s="255"/>
+      <c r="B11" s="279"/>
+      <c r="C11" s="282"/>
       <c r="D11" s="98" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B12" s="253"/>
+      <c r="B12" s="280"/>
       <c r="C12" s="91" t="s">
         <v>61</v>
       </c>
@@ -6086,10 +6068,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:V81"/>
+  <dimension ref="B2:V83"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A4" zoomScale="60" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T58" sqref="T58"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -6114,17 +6096,17 @@
   <sheetData>
     <row r="2" spans="2:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:16" ht="26.25" x14ac:dyDescent="0.3">
-      <c r="B3" s="259" t="s">
-        <v>113</v>
-      </c>
-      <c r="C3" s="260"/>
+      <c r="B3" s="286" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="287"/>
       <c r="D3" s="156"/>
       <c r="E3" s="156"/>
       <c r="F3" s="156"/>
       <c r="G3" s="156"/>
       <c r="H3" s="157"/>
       <c r="J3" s="160" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K3" s="156"/>
       <c r="L3" s="156"/>
@@ -6147,28 +6129,28 @@
       <c r="H5" s="159"/>
       <c r="J5" s="158"/>
       <c r="K5" s="155" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="P5" s="159"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6" s="158"/>
-      <c r="C6" s="256" t="s">
-        <v>217</v>
-      </c>
-      <c r="D6" s="257"/>
-      <c r="E6" s="257"/>
-      <c r="F6" s="257"/>
-      <c r="G6" s="258"/>
+      <c r="C6" s="283" t="s">
+        <v>216</v>
+      </c>
+      <c r="D6" s="284"/>
+      <c r="E6" s="284"/>
+      <c r="F6" s="284"/>
+      <c r="G6" s="285"/>
       <c r="H6" s="159"/>
       <c r="J6" s="158"/>
-      <c r="K6" s="256" t="s">
-        <v>218</v>
-      </c>
-      <c r="L6" s="257"/>
-      <c r="M6" s="257"/>
-      <c r="N6" s="257"/>
-      <c r="O6" s="258"/>
+      <c r="K6" s="283" t="s">
+        <v>217</v>
+      </c>
+      <c r="L6" s="284"/>
+      <c r="M6" s="284"/>
+      <c r="N6" s="284"/>
+      <c r="O6" s="285"/>
       <c r="P6" s="159"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.3">
@@ -6209,14 +6191,16 @@
         <v>87</v>
       </c>
       <c r="D8" s="164" t="s">
+        <v>219</v>
+      </c>
+      <c r="E8" s="164" t="s">
+        <v>83</v>
+      </c>
+      <c r="F8" s="288">
+        <v>0</v>
+      </c>
+      <c r="G8" s="166" t="s">
         <v>220</v>
-      </c>
-      <c r="E8" s="164" t="s">
-        <v>83</v>
-      </c>
-      <c r="F8" s="164"/>
-      <c r="G8" s="166" t="s">
-        <v>221</v>
       </c>
       <c r="H8" s="159"/>
       <c r="J8" s="158"/>
@@ -6224,7 +6208,7 @@
         <v>87</v>
       </c>
       <c r="L8" s="143" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M8" s="143" t="s">
         <v>82</v>
@@ -6233,7 +6217,7 @@
         <v>88</v>
       </c>
       <c r="O8" s="152" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P8" s="159"/>
     </row>
@@ -6255,15 +6239,17 @@
       <c r="H9" s="159"/>
       <c r="J9" s="158"/>
       <c r="K9" s="148"/>
-      <c r="L9" s="261" t="s">
+      <c r="L9" s="139" t="s">
+        <v>219</v>
+      </c>
+      <c r="M9" s="139" t="s">
+        <v>83</v>
+      </c>
+      <c r="N9" s="289">
+        <v>1</v>
+      </c>
+      <c r="O9" s="151" t="s">
         <v>220</v>
-      </c>
-      <c r="M9" s="261" t="s">
-        <v>83</v>
-      </c>
-      <c r="N9" s="261"/>
-      <c r="O9" s="151" t="s">
-        <v>221</v>
       </c>
       <c r="P9" s="159"/>
     </row>
@@ -6408,7 +6394,7 @@
         <v>0</v>
       </c>
       <c r="G14" s="151" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H14" s="159"/>
       <c r="J14" s="158"/>
@@ -6431,7 +6417,7 @@
       <c r="B15" s="158"/>
       <c r="C15" s="137"/>
       <c r="D15" s="139" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E15" s="139" t="s">
         <v>83</v>
@@ -6440,7 +6426,7 @@
         <v>0</v>
       </c>
       <c r="G15" s="151" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H15" s="159"/>
       <c r="J15" s="158"/>
@@ -6455,7 +6441,7 @@
         <v>0</v>
       </c>
       <c r="O15" s="151" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P15" s="159"/>
     </row>
@@ -6463,7 +6449,7 @@
       <c r="B16" s="158"/>
       <c r="C16" s="137"/>
       <c r="D16" s="139" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E16" s="139" t="s">
         <v>83</v>
@@ -6472,13 +6458,13 @@
         <v>0</v>
       </c>
       <c r="G16" s="151" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H16" s="159"/>
       <c r="J16" s="158"/>
       <c r="K16" s="138"/>
       <c r="L16" s="143" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M16" s="143" t="s">
         <v>83</v>
@@ -6487,7 +6473,7 @@
         <v>0</v>
       </c>
       <c r="O16" s="152" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P16" s="159"/>
     </row>
@@ -6495,7 +6481,7 @@
       <c r="B17" s="158"/>
       <c r="C17" s="137"/>
       <c r="D17" s="139" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E17" s="139" t="s">
         <v>95</v>
@@ -6509,7 +6495,7 @@
       <c r="H17" s="159"/>
       <c r="J17" s="158"/>
       <c r="K17" s="162" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M17" s="162">
         <f>ROWS(L8:L16)</f>
@@ -6520,17 +6506,17 @@
     <row r="18" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B18" s="158"/>
       <c r="C18" s="137"/>
-      <c r="D18" s="261" t="s">
-        <v>124</v>
-      </c>
-      <c r="E18" s="261" t="s">
+      <c r="D18" s="139" t="s">
+        <v>123</v>
+      </c>
+      <c r="E18" s="139" t="s">
         <v>95</v>
       </c>
-      <c r="F18" s="264">
+      <c r="F18" s="150">
         <v>0</v>
       </c>
       <c r="G18" s="151" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H18" s="159"/>
       <c r="J18" s="158"/>
@@ -6540,14 +6526,14 @@
     </row>
     <row r="19" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B19" s="158"/>
-      <c r="C19" s="262"/>
-      <c r="D19" s="261" t="s">
+      <c r="C19" s="99"/>
+      <c r="D19" s="139" t="s">
         <v>84</v>
       </c>
-      <c r="E19" s="261" t="s">
+      <c r="E19" s="139" t="s">
         <v>82</v>
       </c>
-      <c r="F19" s="261" t="s">
+      <c r="F19" s="139" t="s">
         <v>88</v>
       </c>
       <c r="G19" s="151" t="s">
@@ -6556,13 +6542,13 @@
       <c r="H19" s="159"/>
       <c r="J19" s="158"/>
       <c r="K19" s="155" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="P19" s="159"/>
     </row>
     <row r="20" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B20" s="158"/>
-      <c r="C20" s="262"/>
+      <c r="C20" s="99"/>
       <c r="D20" s="139" t="s">
         <v>85</v>
       </c>
@@ -6577,23 +6563,23 @@
       </c>
       <c r="H20" s="159"/>
       <c r="J20" s="158"/>
-      <c r="K20" s="256" t="s">
-        <v>219</v>
-      </c>
-      <c r="L20" s="257"/>
-      <c r="M20" s="257"/>
-      <c r="N20" s="257"/>
-      <c r="O20" s="258"/>
+      <c r="K20" s="283" t="s">
+        <v>218</v>
+      </c>
+      <c r="L20" s="284"/>
+      <c r="M20" s="284"/>
+      <c r="N20" s="284"/>
+      <c r="O20" s="285"/>
       <c r="P20" s="159"/>
-      <c r="R20" s="269"/>
-      <c r="S20" s="269"/>
-      <c r="T20" s="269"/>
-      <c r="U20" s="269"/>
-      <c r="V20" s="269"/>
+      <c r="R20" s="168"/>
+      <c r="S20" s="168"/>
+      <c r="T20" s="168"/>
+      <c r="U20" s="168"/>
+      <c r="V20" s="168"/>
     </row>
     <row r="21" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B21" s="158"/>
-      <c r="C21" s="263"/>
+      <c r="C21" s="89"/>
       <c r="D21" s="143" t="s">
         <v>86</v>
       </c>
@@ -6622,16 +6608,16 @@
         <v>78</v>
       </c>
       <c r="P21" s="159"/>
-      <c r="R21" s="269"/>
-      <c r="S21" s="270"/>
-      <c r="T21" s="270"/>
-      <c r="U21" s="270"/>
-      <c r="V21" s="270"/>
+      <c r="R21" s="168"/>
+      <c r="S21" s="169"/>
+      <c r="T21" s="169"/>
+      <c r="U21" s="169"/>
+      <c r="V21" s="169"/>
     </row>
     <row r="22" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B22" s="158"/>
       <c r="C22" s="162" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E22" s="162">
         <f>ROWS(D8:D21)</f>
@@ -6643,7 +6629,7 @@
         <v>87</v>
       </c>
       <c r="L22" s="143" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M22" s="143" t="s">
         <v>82</v>
@@ -6652,50 +6638,46 @@
         <v>88</v>
       </c>
       <c r="O22" s="152" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P22" s="159"/>
-      <c r="R22" s="261"/>
-      <c r="S22" s="261"/>
-      <c r="T22" s="261"/>
-      <c r="U22" s="261"/>
-      <c r="V22" s="266"/>
+      <c r="R22" s="139"/>
+      <c r="S22" s="139"/>
+      <c r="T22" s="139"/>
+      <c r="U22" s="139"/>
+      <c r="V22" s="167"/>
     </row>
     <row r="23" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B23" s="158"/>
       <c r="H23" s="159"/>
       <c r="J23" s="158"/>
       <c r="K23" s="148"/>
-      <c r="L23" s="261" t="s">
+      <c r="L23" s="139" t="s">
+        <v>219</v>
+      </c>
+      <c r="M23" s="139" t="s">
+        <v>83</v>
+      </c>
+      <c r="N23" s="289">
+        <v>1</v>
+      </c>
+      <c r="O23" s="151" t="s">
         <v>220</v>
       </c>
-      <c r="M23" s="261" t="s">
-        <v>83</v>
-      </c>
-      <c r="N23" s="261"/>
-      <c r="O23" s="151" t="s">
-        <v>221</v>
-      </c>
       <c r="P23" s="159"/>
-      <c r="R23" s="261"/>
-      <c r="S23" s="261"/>
-      <c r="T23" s="261"/>
-      <c r="U23" s="261"/>
-      <c r="V23" s="266"/>
+      <c r="R23" s="139"/>
+      <c r="S23" s="139"/>
+      <c r="T23" s="139"/>
+      <c r="U23" s="139"/>
+      <c r="V23" s="167"/>
     </row>
     <row r="24" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B24" s="158"/>
-      <c r="C24" s="271" t="s">
-        <v>112</v>
-      </c>
-      <c r="D24" s="271"/>
-      <c r="E24" s="271"/>
-      <c r="F24" s="271"/>
       <c r="H24" s="159"/>
       <c r="J24" s="158"/>
       <c r="K24" s="137"/>
       <c r="L24" s="139" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="M24" s="139" t="s">
         <v>83</v>
@@ -6704,29 +6686,22 @@
         <v>0</v>
       </c>
       <c r="O24" s="151" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P24" s="159"/>
-      <c r="R24" s="261"/>
-      <c r="S24" s="261"/>
-      <c r="T24" s="261"/>
-      <c r="U24" s="267"/>
-      <c r="V24" s="266"/>
+      <c r="R24" s="139"/>
+      <c r="S24" s="139"/>
+      <c r="T24" s="139"/>
+      <c r="U24" s="141"/>
+      <c r="V24" s="167"/>
     </row>
     <row r="25" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B25" s="158"/>
-      <c r="C25" s="256" t="s">
-        <v>214</v>
-      </c>
-      <c r="D25" s="257"/>
-      <c r="E25" s="257"/>
-      <c r="F25" s="257"/>
-      <c r="G25" s="258"/>
       <c r="H25" s="159"/>
       <c r="J25" s="158"/>
       <c r="K25" s="137"/>
       <c r="L25" s="139" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M25" s="139" t="s">
         <v>83</v>
@@ -6735,35 +6710,27 @@
         <v>0</v>
       </c>
       <c r="O25" s="151" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="P25" s="159"/>
-      <c r="R25" s="268"/>
-      <c r="S25" s="261"/>
-      <c r="T25" s="261"/>
-      <c r="U25" s="267"/>
-      <c r="V25" s="266"/>
+      <c r="S25" s="139"/>
+      <c r="T25" s="139"/>
+      <c r="U25" s="141"/>
+      <c r="V25" s="167"/>
     </row>
     <row r="26" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B26" s="158"/>
-      <c r="C26" s="144"/>
-      <c r="D26" s="145" t="s">
-        <v>97</v>
-      </c>
-      <c r="E26" s="146" t="s">
-        <v>98</v>
-      </c>
-      <c r="F26" s="145" t="s">
-        <v>99</v>
-      </c>
-      <c r="G26" s="147" t="s">
-        <v>78</v>
-      </c>
+      <c r="C26" s="170" t="s">
+        <v>111</v>
+      </c>
+      <c r="D26" s="170"/>
+      <c r="E26" s="170"/>
+      <c r="F26" s="170"/>
       <c r="H26" s="159"/>
       <c r="J26" s="158"/>
       <c r="K26" s="137"/>
       <c r="L26" s="139" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="M26" s="139" t="s">
         <v>95</v>
@@ -6775,34 +6742,25 @@
         <v>104</v>
       </c>
       <c r="P26" s="159"/>
-      <c r="R26" s="268"/>
-      <c r="S26" s="261"/>
-      <c r="T26" s="261"/>
-      <c r="U26" s="267"/>
-      <c r="V26" s="266"/>
+      <c r="S26" s="139"/>
+      <c r="T26" s="139"/>
+      <c r="U26" s="141"/>
+      <c r="V26" s="167"/>
     </row>
     <row r="27" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B27" s="158"/>
-      <c r="C27" s="163" t="s">
-        <v>87</v>
-      </c>
-      <c r="D27" s="164" t="s">
-        <v>105</v>
-      </c>
-      <c r="E27" s="164" t="s">
-        <v>83</v>
-      </c>
-      <c r="F27" s="165">
-        <v>0</v>
-      </c>
-      <c r="G27" s="166" t="s">
-        <v>106</v>
-      </c>
+      <c r="C27" s="283" t="s">
+        <v>213</v>
+      </c>
+      <c r="D27" s="284"/>
+      <c r="E27" s="284"/>
+      <c r="F27" s="284"/>
+      <c r="G27" s="285"/>
       <c r="H27" s="159"/>
       <c r="J27" s="158"/>
       <c r="K27" s="138"/>
       <c r="L27" s="143" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M27" s="143" t="s">
         <v>95</v>
@@ -6811,88 +6769,88 @@
         <v>0</v>
       </c>
       <c r="O27" s="152" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="P27" s="159"/>
-      <c r="R27" s="268"/>
-      <c r="S27" s="261"/>
-      <c r="T27" s="261"/>
-      <c r="U27" s="264"/>
-      <c r="V27" s="266"/>
+      <c r="S27" s="139"/>
+      <c r="T27" s="139"/>
+      <c r="U27" s="150"/>
+      <c r="V27" s="167"/>
     </row>
     <row r="28" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B28" s="158"/>
-      <c r="C28" s="99"/>
-      <c r="D28" s="139" t="s">
-        <v>84</v>
-      </c>
-      <c r="E28" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="F28" s="139" t="s">
-        <v>88</v>
-      </c>
-      <c r="G28" s="151" t="s">
-        <v>79</v>
+      <c r="C28" s="144"/>
+      <c r="D28" s="145" t="s">
+        <v>97</v>
+      </c>
+      <c r="E28" s="146" t="s">
+        <v>98</v>
+      </c>
+      <c r="F28" s="145" t="s">
+        <v>99</v>
+      </c>
+      <c r="G28" s="147" t="s">
+        <v>78</v>
       </c>
       <c r="H28" s="159"/>
       <c r="J28" s="158"/>
       <c r="K28" s="162" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M28" s="162">
         <f>ROWS(L22:L27)</f>
         <v>6</v>
       </c>
       <c r="P28" s="159"/>
-      <c r="R28" s="268"/>
-      <c r="S28" s="261"/>
-      <c r="T28" s="261"/>
-      <c r="U28" s="264"/>
-      <c r="V28" s="266"/>
+      <c r="S28" s="139"/>
+      <c r="T28" s="139"/>
+      <c r="U28" s="150"/>
+      <c r="V28" s="167"/>
     </row>
     <row r="29" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B29" s="158"/>
-      <c r="C29" s="99"/>
-      <c r="D29" s="139" t="s">
-        <v>85</v>
-      </c>
-      <c r="E29" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="F29" s="139" t="s">
-        <v>88</v>
-      </c>
-      <c r="G29" s="151" t="s">
-        <v>80</v>
+      <c r="C29" s="163" t="s">
+        <v>87</v>
+      </c>
+      <c r="D29" s="164" t="s">
+        <v>221</v>
+      </c>
+      <c r="E29" s="164" t="s">
+        <v>83</v>
+      </c>
+      <c r="F29" s="165">
+        <v>1</v>
+      </c>
+      <c r="G29" s="166" t="s">
+        <v>223</v>
       </c>
       <c r="H29" s="159"/>
       <c r="J29" s="158"/>
       <c r="K29" s="155"/>
       <c r="P29" s="159"/>
-      <c r="R29" s="265"/>
-      <c r="S29" s="265"/>
+      <c r="R29" s="155"/>
+      <c r="S29" s="155"/>
       <c r="T29" s="162"/>
     </row>
     <row r="30" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B30" s="158"/>
       <c r="C30" s="99"/>
       <c r="D30" s="139" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E30" s="139" t="s">
-        <v>83</v>
-      </c>
-      <c r="F30" s="141">
-        <v>0</v>
+        <v>82</v>
+      </c>
+      <c r="F30" s="139" t="s">
+        <v>88</v>
       </c>
       <c r="G30" s="151" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H30" s="159"/>
       <c r="J30" s="158"/>
       <c r="K30" s="155" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P30" s="159"/>
     </row>
@@ -6900,42 +6858,42 @@
       <c r="B31" s="158"/>
       <c r="C31" s="99"/>
       <c r="D31" s="139" t="s">
-        <v>167</v>
+        <v>85</v>
       </c>
       <c r="E31" s="139" t="s">
-        <v>83</v>
-      </c>
-      <c r="F31" s="153">
-        <v>0</v>
+        <v>82</v>
+      </c>
+      <c r="F31" s="139" t="s">
+        <v>88</v>
       </c>
       <c r="G31" s="151" t="s">
-        <v>125</v>
+        <v>80</v>
       </c>
       <c r="H31" s="159"/>
       <c r="J31" s="158"/>
-      <c r="K31" s="256" t="s">
-        <v>108</v>
-      </c>
-      <c r="L31" s="257"/>
-      <c r="M31" s="257"/>
-      <c r="N31" s="257"/>
-      <c r="O31" s="258"/>
+      <c r="K31" s="283" t="s">
+        <v>222</v>
+      </c>
+      <c r="L31" s="284"/>
+      <c r="M31" s="284"/>
+      <c r="N31" s="284"/>
+      <c r="O31" s="285"/>
       <c r="P31" s="159"/>
     </row>
     <row r="32" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B32" s="158"/>
-      <c r="C32" s="137"/>
+      <c r="C32" s="99"/>
       <c r="D32" s="139" t="s">
-        <v>189</v>
+        <v>86</v>
       </c>
       <c r="E32" s="139" t="s">
         <v>83</v>
       </c>
-      <c r="F32" s="153">
+      <c r="F32" s="141">
         <v>0</v>
       </c>
       <c r="G32" s="151" t="s">
-        <v>126</v>
+        <v>81</v>
       </c>
       <c r="H32" s="159"/>
       <c r="J32" s="158"/>
@@ -6956,18 +6914,18 @@
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B33" s="158"/>
-      <c r="C33" s="137"/>
+      <c r="C33" s="99"/>
       <c r="D33" s="139" t="s">
-        <v>168</v>
+        <v>105</v>
       </c>
       <c r="E33" s="139" t="s">
         <v>83</v>
       </c>
-      <c r="F33" s="153">
-        <v>0</v>
+      <c r="F33" s="141">
+        <v>1</v>
       </c>
       <c r="G33" s="151" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="H33" s="159"/>
       <c r="J33" s="158"/>
@@ -6975,24 +6933,24 @@
         <v>87</v>
       </c>
       <c r="L33" s="164" t="s">
-        <v>109</v>
+        <v>221</v>
       </c>
       <c r="M33" s="164" t="s">
-        <v>82</v>
-      </c>
-      <c r="N33" s="164" t="s">
-        <v>88</v>
+        <v>83</v>
+      </c>
+      <c r="N33" s="164">
+        <v>1</v>
       </c>
       <c r="O33" s="166" t="s">
-        <v>110</v>
+        <v>223</v>
       </c>
       <c r="P33" s="159"/>
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B34" s="158"/>
-      <c r="C34" s="137"/>
+      <c r="C34" s="99"/>
       <c r="D34" s="139" t="s">
-        <v>190</v>
+        <v>166</v>
       </c>
       <c r="E34" s="139" t="s">
         <v>83</v>
@@ -7001,22 +6959,22 @@
         <v>0</v>
       </c>
       <c r="G34" s="151" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="H34" s="159"/>
       <c r="J34" s="158"/>
-      <c r="K34" s="99"/>
-      <c r="L34" s="139" t="s">
-        <v>167</v>
-      </c>
-      <c r="M34" s="139" t="s">
-        <v>83</v>
-      </c>
-      <c r="N34" s="153">
-        <v>0</v>
+      <c r="K34" s="148"/>
+      <c r="L34" s="290" t="s">
+        <v>108</v>
+      </c>
+      <c r="M34" s="290" t="s">
+        <v>82</v>
+      </c>
+      <c r="N34" s="290" t="s">
+        <v>88</v>
       </c>
       <c r="O34" s="151" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="P34" s="159"/>
     </row>
@@ -7024,7 +6982,7 @@
       <c r="B35" s="158"/>
       <c r="C35" s="137"/>
       <c r="D35" s="139" t="s">
-        <v>169</v>
+        <v>188</v>
       </c>
       <c r="E35" s="139" t="s">
         <v>83</v>
@@ -7033,22 +6991,22 @@
         <v>0</v>
       </c>
       <c r="G35" s="151" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="H35" s="159"/>
       <c r="J35" s="158"/>
-      <c r="K35" s="137"/>
-      <c r="L35" s="139" t="s">
-        <v>189</v>
-      </c>
-      <c r="M35" s="139" t="s">
-        <v>83</v>
-      </c>
-      <c r="N35" s="153">
-        <v>0</v>
+      <c r="K35" s="148"/>
+      <c r="L35" s="290" t="s">
+        <v>105</v>
+      </c>
+      <c r="M35" s="290" t="s">
+        <v>83</v>
+      </c>
+      <c r="N35" s="290">
+        <v>1</v>
       </c>
       <c r="O35" s="151" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="P35" s="159"/>
     </row>
@@ -7056,7 +7014,7 @@
       <c r="B36" s="158"/>
       <c r="C36" s="137"/>
       <c r="D36" s="139" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="E36" s="139" t="s">
         <v>83</v>
@@ -7065,13 +7023,13 @@
         <v>0</v>
       </c>
       <c r="G36" s="151" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="H36" s="159"/>
       <c r="J36" s="158"/>
-      <c r="K36" s="137"/>
+      <c r="K36" s="99"/>
       <c r="L36" s="139" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="M36" s="139" t="s">
         <v>83</v>
@@ -7080,7 +7038,7 @@
         <v>0</v>
       </c>
       <c r="O36" s="151" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="P36" s="159"/>
     </row>
@@ -7088,7 +7046,7 @@
       <c r="B37" s="158"/>
       <c r="C37" s="137"/>
       <c r="D37" s="139" t="s">
-        <v>170</v>
+        <v>189</v>
       </c>
       <c r="E37" s="139" t="s">
         <v>83</v>
@@ -7103,7 +7061,7 @@
       <c r="J37" s="158"/>
       <c r="K37" s="137"/>
       <c r="L37" s="139" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="M37" s="139" t="s">
         <v>83</v>
@@ -7112,7 +7070,7 @@
         <v>0</v>
       </c>
       <c r="O37" s="151" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="P37" s="159"/>
     </row>
@@ -7120,7 +7078,7 @@
       <c r="B38" s="158"/>
       <c r="C38" s="137"/>
       <c r="D38" s="139" t="s">
-        <v>192</v>
+        <v>168</v>
       </c>
       <c r="E38" s="139" t="s">
         <v>83</v>
@@ -7135,7 +7093,7 @@
       <c r="J38" s="158"/>
       <c r="K38" s="137"/>
       <c r="L38" s="139" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="M38" s="139" t="s">
         <v>83</v>
@@ -7144,7 +7102,7 @@
         <v>0</v>
       </c>
       <c r="O38" s="151" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="P38" s="159"/>
     </row>
@@ -7152,7 +7110,7 @@
       <c r="B39" s="158"/>
       <c r="C39" s="137"/>
       <c r="D39" s="139" t="s">
-        <v>171</v>
+        <v>190</v>
       </c>
       <c r="E39" s="139" t="s">
         <v>83</v>
@@ -7161,13 +7119,13 @@
         <v>0</v>
       </c>
       <c r="G39" s="151" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H39" s="159"/>
       <c r="J39" s="158"/>
       <c r="K39" s="137"/>
       <c r="L39" s="139" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="M39" s="139" t="s">
         <v>83</v>
@@ -7176,7 +7134,7 @@
         <v>0</v>
       </c>
       <c r="O39" s="151" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="P39" s="159"/>
     </row>
@@ -7184,7 +7142,7 @@
       <c r="B40" s="158"/>
       <c r="C40" s="137"/>
       <c r="D40" s="139" t="s">
-        <v>193</v>
+        <v>169</v>
       </c>
       <c r="E40" s="139" t="s">
         <v>83</v>
@@ -7193,13 +7151,13 @@
         <v>0</v>
       </c>
       <c r="G40" s="151" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="H40" s="159"/>
       <c r="J40" s="158"/>
       <c r="K40" s="137"/>
       <c r="L40" s="139" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="M40" s="139" t="s">
         <v>83</v>
@@ -7208,7 +7166,7 @@
         <v>0</v>
       </c>
       <c r="O40" s="151" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="P40" s="159"/>
     </row>
@@ -7216,7 +7174,7 @@
       <c r="B41" s="158"/>
       <c r="C41" s="137"/>
       <c r="D41" s="139" t="s">
-        <v>172</v>
+        <v>191</v>
       </c>
       <c r="E41" s="139" t="s">
         <v>83</v>
@@ -7225,13 +7183,13 @@
         <v>0</v>
       </c>
       <c r="G41" s="151" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H41" s="159"/>
       <c r="J41" s="158"/>
       <c r="K41" s="137"/>
       <c r="L41" s="139" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="M41" s="139" t="s">
         <v>83</v>
@@ -7240,7 +7198,7 @@
         <v>0</v>
       </c>
       <c r="O41" s="151" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="P41" s="159"/>
     </row>
@@ -7248,7 +7206,7 @@
       <c r="B42" s="158"/>
       <c r="C42" s="137"/>
       <c r="D42" s="139" t="s">
-        <v>194</v>
+        <v>170</v>
       </c>
       <c r="E42" s="139" t="s">
         <v>83</v>
@@ -7257,13 +7215,13 @@
         <v>0</v>
       </c>
       <c r="G42" s="151" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="H42" s="159"/>
       <c r="J42" s="158"/>
       <c r="K42" s="137"/>
       <c r="L42" s="139" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="M42" s="139" t="s">
         <v>83</v>
@@ -7272,7 +7230,7 @@
         <v>0</v>
       </c>
       <c r="O42" s="151" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="P42" s="159"/>
     </row>
@@ -7280,7 +7238,7 @@
       <c r="B43" s="158"/>
       <c r="C43" s="137"/>
       <c r="D43" s="139" t="s">
-        <v>173</v>
+        <v>192</v>
       </c>
       <c r="E43" s="139" t="s">
         <v>83</v>
@@ -7295,7 +7253,7 @@
       <c r="J43" s="158"/>
       <c r="K43" s="137"/>
       <c r="L43" s="139" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="M43" s="139" t="s">
         <v>83</v>
@@ -7304,7 +7262,7 @@
         <v>0</v>
       </c>
       <c r="O43" s="151" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="P43" s="159"/>
     </row>
@@ -7312,7 +7270,7 @@
       <c r="B44" s="158"/>
       <c r="C44" s="137"/>
       <c r="D44" s="139" t="s">
-        <v>195</v>
+        <v>171</v>
       </c>
       <c r="E44" s="139" t="s">
         <v>83</v>
@@ -7327,7 +7285,7 @@
       <c r="J44" s="158"/>
       <c r="K44" s="137"/>
       <c r="L44" s="139" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="M44" s="139" t="s">
         <v>83</v>
@@ -7336,7 +7294,7 @@
         <v>0</v>
       </c>
       <c r="O44" s="151" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="P44" s="159"/>
     </row>
@@ -7344,7 +7302,7 @@
       <c r="B45" s="158"/>
       <c r="C45" s="137"/>
       <c r="D45" s="139" t="s">
-        <v>174</v>
+        <v>193</v>
       </c>
       <c r="E45" s="139" t="s">
         <v>83</v>
@@ -7353,13 +7311,13 @@
         <v>0</v>
       </c>
       <c r="G45" s="151" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H45" s="159"/>
       <c r="J45" s="158"/>
       <c r="K45" s="137"/>
       <c r="L45" s="139" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="M45" s="139" t="s">
         <v>83</v>
@@ -7368,15 +7326,15 @@
         <v>0</v>
       </c>
       <c r="O45" s="151" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P45" s="159"/>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B46" s="158"/>
-      <c r="C46" s="148"/>
+      <c r="C46" s="137"/>
       <c r="D46" s="139" t="s">
-        <v>196</v>
+        <v>172</v>
       </c>
       <c r="E46" s="139" t="s">
         <v>83</v>
@@ -7385,13 +7343,13 @@
         <v>0</v>
       </c>
       <c r="G46" s="151" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="H46" s="159"/>
       <c r="J46" s="158"/>
       <c r="K46" s="137"/>
       <c r="L46" s="139" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="M46" s="139" t="s">
         <v>83</v>
@@ -7400,7 +7358,7 @@
         <v>0</v>
       </c>
       <c r="O46" s="151" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="P46" s="159"/>
     </row>
@@ -7408,7 +7366,7 @@
       <c r="B47" s="158"/>
       <c r="C47" s="137"/>
       <c r="D47" s="139" t="s">
-        <v>175</v>
+        <v>194</v>
       </c>
       <c r="E47" s="139" t="s">
         <v>83</v>
@@ -7417,13 +7375,13 @@
         <v>0</v>
       </c>
       <c r="G47" s="151" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="H47" s="159"/>
       <c r="J47" s="158"/>
       <c r="K47" s="137"/>
       <c r="L47" s="139" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="M47" s="139" t="s">
         <v>83</v>
@@ -7432,15 +7390,15 @@
         <v>0</v>
       </c>
       <c r="O47" s="151" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="P47" s="159"/>
     </row>
     <row r="48" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B48" s="158"/>
-      <c r="C48" s="148"/>
+      <c r="C48" s="137"/>
       <c r="D48" s="139" t="s">
-        <v>197</v>
+        <v>173</v>
       </c>
       <c r="E48" s="139" t="s">
         <v>83</v>
@@ -7449,13 +7407,13 @@
         <v>0</v>
       </c>
       <c r="G48" s="151" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="H48" s="159"/>
       <c r="J48" s="158"/>
       <c r="K48" s="137"/>
       <c r="L48" s="139" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="M48" s="139" t="s">
         <v>83</v>
@@ -7464,15 +7422,15 @@
         <v>0</v>
       </c>
       <c r="O48" s="151" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="P48" s="159"/>
     </row>
     <row r="49" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B49" s="158"/>
-      <c r="C49" s="137"/>
+      <c r="C49" s="148"/>
       <c r="D49" s="139" t="s">
-        <v>176</v>
+        <v>195</v>
       </c>
       <c r="E49" s="139" t="s">
         <v>83</v>
@@ -7481,13 +7439,13 @@
         <v>0</v>
       </c>
       <c r="G49" s="151" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="H49" s="159"/>
       <c r="J49" s="158"/>
       <c r="K49" s="137"/>
       <c r="L49" s="139" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="M49" s="139" t="s">
         <v>83</v>
@@ -7496,15 +7454,15 @@
         <v>0</v>
       </c>
       <c r="O49" s="151" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="P49" s="159"/>
     </row>
     <row r="50" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B50" s="158"/>
-      <c r="C50" s="148"/>
+      <c r="C50" s="137"/>
       <c r="D50" s="139" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
       <c r="E50" s="139" t="s">
         <v>83</v>
@@ -7513,13 +7471,13 @@
         <v>0</v>
       </c>
       <c r="G50" s="151" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="H50" s="159"/>
       <c r="J50" s="158"/>
-      <c r="K50" s="148"/>
+      <c r="K50" s="137"/>
       <c r="L50" s="139" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="M50" s="139" t="s">
         <v>83</v>
@@ -7528,15 +7486,15 @@
         <v>0</v>
       </c>
       <c r="O50" s="151" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="P50" s="159"/>
     </row>
     <row r="51" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B51" s="158"/>
-      <c r="C51" s="137"/>
+      <c r="C51" s="148"/>
       <c r="D51" s="139" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
       <c r="E51" s="139" t="s">
         <v>83</v>
@@ -7545,13 +7503,13 @@
         <v>0</v>
       </c>
       <c r="G51" s="151" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="H51" s="159"/>
       <c r="J51" s="161"/>
       <c r="K51" s="137"/>
       <c r="L51" s="139" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="M51" s="139" t="s">
         <v>83</v>
@@ -7560,15 +7518,15 @@
         <v>0</v>
       </c>
       <c r="O51" s="151" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="P51" s="159"/>
     </row>
     <row r="52" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B52" s="158"/>
-      <c r="C52" s="148"/>
+      <c r="C52" s="137"/>
       <c r="D52" s="139" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
       <c r="E52" s="139" t="s">
         <v>83</v>
@@ -7577,13 +7535,13 @@
         <v>0</v>
       </c>
       <c r="G52" s="151" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H52" s="159"/>
       <c r="J52" s="158"/>
       <c r="K52" s="148"/>
       <c r="L52" s="139" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="M52" s="139" t="s">
         <v>83</v>
@@ -7592,15 +7550,15 @@
         <v>0</v>
       </c>
       <c r="O52" s="151" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="P52" s="159"/>
     </row>
     <row r="53" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B53" s="158"/>
-      <c r="C53" s="137"/>
+      <c r="C53" s="148"/>
       <c r="D53" s="139" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
       <c r="E53" s="139" t="s">
         <v>83</v>
@@ -7608,14 +7566,14 @@
       <c r="F53" s="153">
         <v>0</v>
       </c>
-      <c r="G53" s="135" t="s">
-        <v>143</v>
+      <c r="G53" s="151" t="s">
+        <v>139</v>
       </c>
       <c r="H53" s="159"/>
       <c r="J53" s="158"/>
       <c r="K53" s="137"/>
       <c r="L53" s="139" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="M53" s="139" t="s">
         <v>83</v>
@@ -7624,7 +7582,7 @@
         <v>0</v>
       </c>
       <c r="O53" s="151" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="P53" s="159"/>
     </row>
@@ -7632,7 +7590,7 @@
       <c r="B54" s="158"/>
       <c r="C54" s="137"/>
       <c r="D54" s="139" t="s">
-        <v>210</v>
+        <v>176</v>
       </c>
       <c r="E54" s="139" t="s">
         <v>83</v>
@@ -7640,14 +7598,14 @@
       <c r="F54" s="153">
         <v>0</v>
       </c>
-      <c r="G54" s="135" t="s">
-        <v>144</v>
+      <c r="G54" s="151" t="s">
+        <v>140</v>
       </c>
       <c r="H54" s="159"/>
       <c r="J54" s="158"/>
       <c r="K54" s="148"/>
       <c r="L54" s="139" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="M54" s="139" t="s">
         <v>83</v>
@@ -7656,15 +7614,15 @@
         <v>0</v>
       </c>
       <c r="O54" s="151" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="P54" s="159"/>
     </row>
     <row r="55" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B55" s="158"/>
-      <c r="C55" s="137"/>
+      <c r="C55" s="148"/>
       <c r="D55" s="139" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="E55" s="139" t="s">
         <v>83</v>
@@ -7672,14 +7630,14 @@
       <c r="F55" s="153">
         <v>0</v>
       </c>
-      <c r="G55" s="135" t="s">
-        <v>145</v>
+      <c r="G55" s="151" t="s">
+        <v>141</v>
       </c>
       <c r="H55" s="159"/>
       <c r="J55" s="158"/>
       <c r="K55" s="137"/>
       <c r="L55" s="139" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="M55" s="139" t="s">
         <v>83</v>
@@ -7688,7 +7646,7 @@
         <v>0</v>
       </c>
       <c r="O55" s="151" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="P55" s="159"/>
     </row>
@@ -7705,13 +7663,13 @@
         <v>0</v>
       </c>
       <c r="G56" s="135" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="H56" s="159"/>
       <c r="J56" s="158"/>
       <c r="K56" s="148"/>
       <c r="L56" s="139" t="s">
-        <v>213</v>
+        <v>176</v>
       </c>
       <c r="M56" s="139" t="s">
         <v>83</v>
@@ -7719,8 +7677,8 @@
       <c r="N56" s="153">
         <v>0</v>
       </c>
-      <c r="O56" s="135" t="s">
-        <v>143</v>
+      <c r="O56" s="151" t="s">
+        <v>140</v>
       </c>
       <c r="P56" s="159"/>
     </row>
@@ -7728,7 +7686,7 @@
       <c r="B57" s="158"/>
       <c r="C57" s="137"/>
       <c r="D57" s="139" t="s">
-        <v>178</v>
+        <v>209</v>
       </c>
       <c r="E57" s="139" t="s">
         <v>83</v>
@@ -7737,13 +7695,13 @@
         <v>0</v>
       </c>
       <c r="G57" s="135" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="H57" s="159"/>
       <c r="J57" s="158"/>
       <c r="K57" s="137"/>
       <c r="L57" s="139" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="M57" s="139" t="s">
         <v>83</v>
@@ -7751,8 +7709,8 @@
       <c r="N57" s="153">
         <v>0</v>
       </c>
-      <c r="O57" s="135" t="s">
-        <v>144</v>
+      <c r="O57" s="151" t="s">
+        <v>141</v>
       </c>
       <c r="P57" s="159"/>
     </row>
@@ -7760,7 +7718,7 @@
       <c r="B58" s="158"/>
       <c r="C58" s="137"/>
       <c r="D58" s="139" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="E58" s="139" t="s">
         <v>83</v>
@@ -7769,13 +7727,13 @@
         <v>0</v>
       </c>
       <c r="G58" s="135" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H58" s="159"/>
       <c r="J58" s="158"/>
-      <c r="K58" s="137"/>
+      <c r="K58" s="148"/>
       <c r="L58" s="139" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="M58" s="139" t="s">
         <v>83</v>
@@ -7784,7 +7742,7 @@
         <v>0</v>
       </c>
       <c r="O58" s="135" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="P58" s="159"/>
     </row>
@@ -7792,7 +7750,7 @@
       <c r="B59" s="158"/>
       <c r="C59" s="137"/>
       <c r="D59" s="139" t="s">
-        <v>179</v>
+        <v>211</v>
       </c>
       <c r="E59" s="139" t="s">
         <v>83</v>
@@ -7801,13 +7759,13 @@
         <v>0</v>
       </c>
       <c r="G59" s="135" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H59" s="159"/>
       <c r="J59" s="158"/>
       <c r="K59" s="137"/>
       <c r="L59" s="139" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="M59" s="139" t="s">
         <v>83</v>
@@ -7816,7 +7774,7 @@
         <v>0</v>
       </c>
       <c r="O59" s="135" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="P59" s="159"/>
     </row>
@@ -7824,7 +7782,7 @@
       <c r="B60" s="158"/>
       <c r="C60" s="137"/>
       <c r="D60" s="139" t="s">
-        <v>201</v>
+        <v>177</v>
       </c>
       <c r="E60" s="139" t="s">
         <v>83</v>
@@ -7833,13 +7791,13 @@
         <v>0</v>
       </c>
       <c r="G60" s="135" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H60" s="159"/>
       <c r="J60" s="158"/>
       <c r="K60" s="137"/>
       <c r="L60" s="139" t="s">
-        <v>178</v>
+        <v>210</v>
       </c>
       <c r="M60" s="139" t="s">
         <v>83</v>
@@ -7848,7 +7806,7 @@
         <v>0</v>
       </c>
       <c r="O60" s="135" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="P60" s="159"/>
     </row>
@@ -7856,7 +7814,7 @@
       <c r="B61" s="158"/>
       <c r="C61" s="137"/>
       <c r="D61" s="139" t="s">
-        <v>180</v>
+        <v>199</v>
       </c>
       <c r="E61" s="139" t="s">
         <v>83</v>
@@ -7865,13 +7823,13 @@
         <v>0</v>
       </c>
       <c r="G61" s="135" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="H61" s="159"/>
       <c r="J61" s="158"/>
       <c r="K61" s="137"/>
       <c r="L61" s="139" t="s">
-        <v>200</v>
+        <v>211</v>
       </c>
       <c r="M61" s="139" t="s">
         <v>83</v>
@@ -7880,7 +7838,7 @@
         <v>0</v>
       </c>
       <c r="O61" s="135" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="P61" s="159"/>
     </row>
@@ -7888,7 +7846,7 @@
       <c r="B62" s="158"/>
       <c r="C62" s="137"/>
       <c r="D62" s="139" t="s">
-        <v>202</v>
+        <v>178</v>
       </c>
       <c r="E62" s="139" t="s">
         <v>83</v>
@@ -7897,13 +7855,13 @@
         <v>0</v>
       </c>
       <c r="G62" s="135" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="H62" s="159"/>
       <c r="J62" s="158"/>
       <c r="K62" s="137"/>
       <c r="L62" s="139" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M62" s="139" t="s">
         <v>83</v>
@@ -7912,7 +7870,7 @@
         <v>0</v>
       </c>
       <c r="O62" s="135" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="P62" s="159"/>
     </row>
@@ -7920,7 +7878,7 @@
       <c r="B63" s="158"/>
       <c r="C63" s="137"/>
       <c r="D63" s="139" t="s">
-        <v>181</v>
+        <v>200</v>
       </c>
       <c r="E63" s="139" t="s">
         <v>83</v>
@@ -7929,13 +7887,13 @@
         <v>0</v>
       </c>
       <c r="G63" s="135" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="H63" s="159"/>
       <c r="J63" s="158"/>
       <c r="K63" s="137"/>
       <c r="L63" s="139" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="M63" s="139" t="s">
         <v>83</v>
@@ -7944,7 +7902,7 @@
         <v>0</v>
       </c>
       <c r="O63" s="135" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="P63" s="159"/>
     </row>
@@ -7952,7 +7910,7 @@
       <c r="B64" s="158"/>
       <c r="C64" s="137"/>
       <c r="D64" s="139" t="s">
-        <v>203</v>
+        <v>179</v>
       </c>
       <c r="E64" s="139" t="s">
         <v>83</v>
@@ -7961,13 +7919,13 @@
         <v>0</v>
       </c>
       <c r="G64" s="135" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H64" s="159"/>
       <c r="J64" s="158"/>
       <c r="K64" s="137"/>
       <c r="L64" s="139" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="M64" s="139" t="s">
         <v>83</v>
@@ -7976,7 +7934,7 @@
         <v>0</v>
       </c>
       <c r="O64" s="135" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="P64" s="159"/>
     </row>
@@ -7984,7 +7942,7 @@
       <c r="B65" s="158"/>
       <c r="C65" s="137"/>
       <c r="D65" s="139" t="s">
-        <v>182</v>
+        <v>201</v>
       </c>
       <c r="E65" s="139" t="s">
         <v>83</v>
@@ -7993,13 +7951,13 @@
         <v>0</v>
       </c>
       <c r="G65" s="135" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="H65" s="159"/>
       <c r="J65" s="158"/>
       <c r="K65" s="137"/>
       <c r="L65" s="139" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="M65" s="139" t="s">
         <v>83</v>
@@ -8008,7 +7966,7 @@
         <v>0</v>
       </c>
       <c r="O65" s="135" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="P65" s="159"/>
     </row>
@@ -8016,7 +7974,7 @@
       <c r="B66" s="158"/>
       <c r="C66" s="137"/>
       <c r="D66" s="139" t="s">
-        <v>204</v>
+        <v>180</v>
       </c>
       <c r="E66" s="139" t="s">
         <v>83</v>
@@ -8025,13 +7983,13 @@
         <v>0</v>
       </c>
       <c r="G66" s="135" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="H66" s="159"/>
       <c r="J66" s="158"/>
       <c r="K66" s="137"/>
       <c r="L66" s="139" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="M66" s="139" t="s">
         <v>83</v>
@@ -8040,7 +7998,7 @@
         <v>0</v>
       </c>
       <c r="O66" s="135" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="P66" s="159"/>
     </row>
@@ -8048,7 +8006,7 @@
       <c r="B67" s="158"/>
       <c r="C67" s="137"/>
       <c r="D67" s="139" t="s">
-        <v>183</v>
+        <v>202</v>
       </c>
       <c r="E67" s="139" t="s">
         <v>83</v>
@@ -8057,13 +8015,13 @@
         <v>0</v>
       </c>
       <c r="G67" s="135" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="H67" s="159"/>
       <c r="J67" s="158"/>
       <c r="K67" s="137"/>
       <c r="L67" s="139" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="M67" s="139" t="s">
         <v>83</v>
@@ -8072,7 +8030,7 @@
         <v>0</v>
       </c>
       <c r="O67" s="135" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="P67" s="159"/>
     </row>
@@ -8080,7 +8038,7 @@
       <c r="B68" s="158"/>
       <c r="C68" s="137"/>
       <c r="D68" s="139" t="s">
-        <v>205</v>
+        <v>181</v>
       </c>
       <c r="E68" s="139" t="s">
         <v>83</v>
@@ -8089,13 +8047,13 @@
         <v>0</v>
       </c>
       <c r="G68" s="135" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="H68" s="159"/>
       <c r="J68" s="158"/>
       <c r="K68" s="137"/>
       <c r="L68" s="139" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="M68" s="139" t="s">
         <v>83</v>
@@ -8104,7 +8062,7 @@
         <v>0</v>
       </c>
       <c r="O68" s="135" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="P68" s="159"/>
     </row>
@@ -8112,7 +8070,7 @@
       <c r="B69" s="158"/>
       <c r="C69" s="137"/>
       <c r="D69" s="139" t="s">
-        <v>184</v>
+        <v>203</v>
       </c>
       <c r="E69" s="139" t="s">
         <v>83</v>
@@ -8121,13 +8079,13 @@
         <v>0</v>
       </c>
       <c r="G69" s="135" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="H69" s="159"/>
       <c r="J69" s="158"/>
       <c r="K69" s="137"/>
       <c r="L69" s="139" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="M69" s="139" t="s">
         <v>83</v>
@@ -8136,7 +8094,7 @@
         <v>0</v>
       </c>
       <c r="O69" s="135" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="P69" s="159"/>
     </row>
@@ -8144,7 +8102,7 @@
       <c r="B70" s="158"/>
       <c r="C70" s="137"/>
       <c r="D70" s="139" t="s">
-        <v>206</v>
+        <v>182</v>
       </c>
       <c r="E70" s="139" t="s">
         <v>83</v>
@@ -8153,13 +8111,13 @@
         <v>0</v>
       </c>
       <c r="G70" s="135" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="H70" s="159"/>
       <c r="J70" s="158"/>
       <c r="K70" s="137"/>
       <c r="L70" s="139" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="M70" s="139" t="s">
         <v>83</v>
@@ -8168,7 +8126,7 @@
         <v>0</v>
       </c>
       <c r="O70" s="135" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="P70" s="159"/>
     </row>
@@ -8176,7 +8134,7 @@
       <c r="B71" s="158"/>
       <c r="C71" s="137"/>
       <c r="D71" s="139" t="s">
-        <v>185</v>
+        <v>204</v>
       </c>
       <c r="E71" s="139" t="s">
         <v>83</v>
@@ -8185,13 +8143,13 @@
         <v>0</v>
       </c>
       <c r="G71" s="135" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H71" s="159"/>
       <c r="J71" s="158"/>
       <c r="K71" s="137"/>
       <c r="L71" s="139" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="M71" s="139" t="s">
         <v>83</v>
@@ -8200,7 +8158,7 @@
         <v>0</v>
       </c>
       <c r="O71" s="135" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="P71" s="159"/>
     </row>
@@ -8208,7 +8166,7 @@
       <c r="B72" s="158"/>
       <c r="C72" s="137"/>
       <c r="D72" s="139" t="s">
-        <v>207</v>
+        <v>183</v>
       </c>
       <c r="E72" s="139" t="s">
         <v>83</v>
@@ -8217,13 +8175,13 @@
         <v>0</v>
       </c>
       <c r="G72" s="135" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="H72" s="159"/>
       <c r="J72" s="158"/>
       <c r="K72" s="137"/>
       <c r="L72" s="139" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M72" s="139" t="s">
         <v>83</v>
@@ -8232,7 +8190,7 @@
         <v>0</v>
       </c>
       <c r="O72" s="135" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="P72" s="159"/>
     </row>
@@ -8240,7 +8198,7 @@
       <c r="B73" s="158"/>
       <c r="C73" s="137"/>
       <c r="D73" s="139" t="s">
-        <v>186</v>
+        <v>205</v>
       </c>
       <c r="E73" s="139" t="s">
         <v>83</v>
@@ -8249,13 +8207,13 @@
         <v>0</v>
       </c>
       <c r="G73" s="135" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H73" s="159"/>
       <c r="J73" s="158"/>
       <c r="K73" s="137"/>
       <c r="L73" s="139" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="M73" s="139" t="s">
         <v>83</v>
@@ -8264,7 +8222,7 @@
         <v>0</v>
       </c>
       <c r="O73" s="135" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="P73" s="159"/>
     </row>
@@ -8272,7 +8230,7 @@
       <c r="B74" s="158"/>
       <c r="C74" s="137"/>
       <c r="D74" s="139" t="s">
-        <v>208</v>
+        <v>184</v>
       </c>
       <c r="E74" s="139" t="s">
         <v>83</v>
@@ -8281,13 +8239,13 @@
         <v>0</v>
       </c>
       <c r="G74" s="135" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="H74" s="159"/>
       <c r="J74" s="158"/>
       <c r="K74" s="137"/>
       <c r="L74" s="139" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="M74" s="139" t="s">
         <v>83</v>
@@ -8296,7 +8254,7 @@
         <v>0</v>
       </c>
       <c r="O74" s="135" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="P74" s="159"/>
     </row>
@@ -8304,7 +8262,7 @@
       <c r="B75" s="158"/>
       <c r="C75" s="137"/>
       <c r="D75" s="139" t="s">
-        <v>187</v>
+        <v>206</v>
       </c>
       <c r="E75" s="139" t="s">
         <v>83</v>
@@ -8313,13 +8271,13 @@
         <v>0</v>
       </c>
       <c r="G75" s="135" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="H75" s="159"/>
       <c r="J75" s="158"/>
       <c r="K75" s="137"/>
       <c r="L75" s="139" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="M75" s="139" t="s">
         <v>83</v>
@@ -8328,30 +8286,30 @@
         <v>0</v>
       </c>
       <c r="O75" s="135" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="P75" s="159"/>
     </row>
     <row r="76" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B76" s="158"/>
-      <c r="C76" s="138"/>
-      <c r="D76" s="134" t="s">
-        <v>188</v>
-      </c>
-      <c r="E76" s="143" t="s">
-        <v>83</v>
-      </c>
-      <c r="F76" s="154">
-        <v>0</v>
-      </c>
-      <c r="G76" s="136" t="s">
-        <v>166</v>
+      <c r="C76" s="137"/>
+      <c r="D76" s="139" t="s">
+        <v>185</v>
+      </c>
+      <c r="E76" s="139" t="s">
+        <v>83</v>
+      </c>
+      <c r="F76" s="153">
+        <v>0</v>
+      </c>
+      <c r="G76" s="135" t="s">
+        <v>162</v>
       </c>
       <c r="H76" s="159"/>
       <c r="J76" s="158"/>
       <c r="K76" s="137"/>
       <c r="L76" s="139" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="M76" s="139" t="s">
         <v>83</v>
@@ -8360,24 +8318,30 @@
         <v>0</v>
       </c>
       <c r="O76" s="135" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="P76" s="159"/>
     </row>
     <row r="77" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B77" s="158"/>
-      <c r="C77" s="155" t="s">
-        <v>115</v>
-      </c>
-      <c r="E77" s="162">
-        <f>ROWS(D27:D76)</f>
-        <v>50</v>
+      <c r="C77" s="137"/>
+      <c r="D77" s="139" t="s">
+        <v>207</v>
+      </c>
+      <c r="E77" s="139" t="s">
+        <v>83</v>
+      </c>
+      <c r="F77" s="153">
+        <v>0</v>
+      </c>
+      <c r="G77" s="135" t="s">
+        <v>163</v>
       </c>
       <c r="H77" s="159"/>
       <c r="J77" s="158"/>
       <c r="K77" s="137"/>
       <c r="L77" s="139" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="M77" s="139" t="s">
         <v>83</v>
@@ -8386,19 +8350,30 @@
         <v>0</v>
       </c>
       <c r="O77" s="135" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="P77" s="159"/>
     </row>
     <row r="78" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B78" s="158"/>
-      <c r="C78" s="268"/>
-      <c r="G78" s="268"/>
+      <c r="C78" s="137"/>
+      <c r="D78" s="139" t="s">
+        <v>186</v>
+      </c>
+      <c r="E78" s="139" t="s">
+        <v>83</v>
+      </c>
+      <c r="F78" s="153">
+        <v>0</v>
+      </c>
+      <c r="G78" s="135" t="s">
+        <v>164</v>
+      </c>
       <c r="H78" s="159"/>
       <c r="J78" s="158"/>
       <c r="K78" s="137"/>
       <c r="L78" s="139" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="M78" s="139" t="s">
         <v>83</v>
@@ -8407,57 +8382,115 @@
         <v>0</v>
       </c>
       <c r="O78" s="135" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="P78" s="159"/>
     </row>
     <row r="79" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B79" s="158"/>
+      <c r="C79" s="138"/>
+      <c r="D79" s="134" t="s">
+        <v>187</v>
+      </c>
+      <c r="E79" s="143" t="s">
+        <v>83</v>
+      </c>
+      <c r="F79" s="154">
+        <v>0</v>
+      </c>
+      <c r="G79" s="136" t="s">
+        <v>165</v>
+      </c>
       <c r="H79" s="159"/>
       <c r="J79" s="158"/>
-      <c r="K79" s="138"/>
-      <c r="L79" s="134" t="s">
-        <v>188</v>
-      </c>
-      <c r="M79" s="143" t="s">
-        <v>83</v>
-      </c>
-      <c r="N79" s="154">
-        <v>0</v>
-      </c>
-      <c r="O79" s="136" t="s">
-        <v>166</v>
+      <c r="K79" s="137"/>
+      <c r="L79" s="139" t="s">
+        <v>207</v>
+      </c>
+      <c r="M79" s="139" t="s">
+        <v>83</v>
+      </c>
+      <c r="N79" s="153">
+        <v>0</v>
+      </c>
+      <c r="O79" s="135" t="s">
+        <v>163</v>
       </c>
       <c r="P79" s="159"/>
     </row>
     <row r="80" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B80" s="158"/>
+      <c r="C80" s="155" t="s">
+        <v>114</v>
+      </c>
+      <c r="E80" s="162">
+        <f>ROWS(D29:D79)</f>
+        <v>51</v>
+      </c>
       <c r="H80" s="159"/>
       <c r="J80" s="158"/>
-      <c r="K80" s="155" t="s">
-        <v>115</v>
-      </c>
-      <c r="M80" s="162">
-        <f>ROWS(L33:L79)</f>
-        <v>47</v>
+      <c r="K80" s="137"/>
+      <c r="L80" s="139" t="s">
+        <v>186</v>
+      </c>
+      <c r="M80" s="139" t="s">
+        <v>83</v>
+      </c>
+      <c r="N80" s="153">
+        <v>0</v>
+      </c>
+      <c r="O80" s="135" t="s">
+        <v>164</v>
       </c>
       <c r="P80" s="159"/>
     </row>
-    <row r="81" spans="2:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B81" s="272"/>
-      <c r="C81" s="273"/>
-      <c r="D81" s="273"/>
-      <c r="E81" s="273"/>
-      <c r="F81" s="273"/>
-      <c r="G81" s="273"/>
-      <c r="H81" s="274"/>
-      <c r="J81" s="272"/>
-      <c r="K81" s="273"/>
-      <c r="L81" s="273"/>
-      <c r="M81" s="273"/>
-      <c r="N81" s="273"/>
-      <c r="O81" s="273"/>
-      <c r="P81" s="274"/>
+    <row r="81" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B81" s="158"/>
+      <c r="H81" s="159"/>
+      <c r="J81" s="158"/>
+      <c r="K81" s="138"/>
+      <c r="L81" s="134" t="s">
+        <v>187</v>
+      </c>
+      <c r="M81" s="143" t="s">
+        <v>83</v>
+      </c>
+      <c r="N81" s="154">
+        <v>0</v>
+      </c>
+      <c r="O81" s="136" t="s">
+        <v>165</v>
+      </c>
+      <c r="P81" s="159"/>
+    </row>
+    <row r="82" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B82" s="158"/>
+      <c r="H82" s="159"/>
+      <c r="J82" s="158"/>
+      <c r="K82" s="155" t="s">
+        <v>114</v>
+      </c>
+      <c r="M82" s="162">
+        <f>ROWS(L33:L81)</f>
+        <v>49</v>
+      </c>
+      <c r="P82" s="159"/>
+    </row>
+    <row r="83" spans="2:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B83" s="171"/>
+      <c r="C83" s="172"/>
+      <c r="D83" s="172"/>
+      <c r="E83" s="172"/>
+      <c r="F83" s="172"/>
+      <c r="G83" s="172"/>
+      <c r="H83" s="173"/>
+      <c r="J83" s="171"/>
+      <c r="K83" s="172"/>
+      <c r="L83" s="172"/>
+      <c r="M83" s="172"/>
+      <c r="N83" s="172"/>
+      <c r="O83" s="172"/>
+      <c r="P83" s="173"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -8466,7 +8499,7 @@
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="C6:G6"/>
     <mergeCell ref="K6:O6"/>
-    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C27:G27"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>